<commit_message>
Added the columns supervisor, contact...
</commit_message>
<xml_diff>
--- a/Data/TS_2016_data.xlsx
+++ b/Data/TS_2016_data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="202">
   <si>
     <t>Date</t>
   </si>
@@ -135,9 +135,6 @@
     <t>MEVYANN</t>
   </si>
   <si>
-    <t>Rhett  Chester</t>
-  </si>
-  <si>
     <t>MFOUMBI IBINGA</t>
   </si>
   <si>
@@ -619,6 +616,18 @@
   </si>
   <si>
     <t>P</t>
+  </si>
+  <si>
+    <t>Rhett Chester</t>
+  </si>
+  <si>
+    <t>Supervisor</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Full-Time</t>
   </si>
 </sst>
 </file>
@@ -1179,7 +1188,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1255,12 +1264,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ80"/>
+  <dimension ref="A1:AML80"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1268,16 +1277,18 @@
     <col min="1" max="1" width="10.7109375"/>
     <col min="2" max="2" width="28.85546875" style="6"/>
     <col min="3" max="3" width="21.85546875" style="6"/>
-    <col min="4" max="4" width="10.5703125" style="6"/>
-    <col min="5" max="5" width="11" style="6"/>
-    <col min="6" max="14" width="2" style="7" customWidth="1"/>
-    <col min="15" max="15" width="3" style="7" customWidth="1"/>
-    <col min="16" max="36" width="3" style="7" bestFit="1" customWidth="1"/>
-    <col min="38" max="1020" width="10.85546875" style="6"/>
-    <col min="1021" max="1025" width="10.85546875"/>
+    <col min="4" max="4" width="21.140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="6"/>
+    <col min="6" max="6" width="9.140625" style="6"/>
+    <col min="7" max="7" width="11" style="6"/>
+    <col min="8" max="16" width="2" style="7" customWidth="1"/>
+    <col min="17" max="17" width="3" style="7" customWidth="1"/>
+    <col min="18" max="38" width="3" style="7" bestFit="1" customWidth="1"/>
+    <col min="40" max="1022" width="10.85546875" style="6"/>
+    <col min="1023" max="1027" width="10.85546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1026" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
@@ -1288,119 +1299,125 @@
         <v>30</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="8">
+      <c r="H1" s="8">
         <v>1</v>
       </c>
-      <c r="G1" s="8">
+      <c r="I1" s="8">
         <v>2</v>
       </c>
-      <c r="H1" s="8">
+      <c r="J1" s="8">
         <v>3</v>
       </c>
-      <c r="I1" s="8">
+      <c r="K1" s="8">
         <v>4</v>
       </c>
-      <c r="J1" s="8">
+      <c r="L1" s="8">
         <v>5</v>
       </c>
-      <c r="K1" s="8">
+      <c r="M1" s="8">
         <v>6</v>
       </c>
-      <c r="L1" s="8">
+      <c r="N1" s="8">
         <v>7</v>
       </c>
-      <c r="M1" s="8">
-        <v>8</v>
-      </c>
-      <c r="N1" s="8">
+      <c r="O1" s="8">
+        <v>8</v>
+      </c>
+      <c r="P1" s="8">
         <v>9</v>
       </c>
-      <c r="O1" s="8">
+      <c r="Q1" s="8">
         <v>10</v>
       </c>
-      <c r="P1" s="8">
+      <c r="R1" s="8">
         <v>11</v>
       </c>
-      <c r="Q1" s="8">
+      <c r="S1" s="8">
         <v>12</v>
       </c>
-      <c r="R1" s="8">
+      <c r="T1" s="8">
         <v>13</v>
       </c>
-      <c r="S1" s="8">
+      <c r="U1" s="8">
         <v>14</v>
       </c>
-      <c r="T1" s="8">
+      <c r="V1" s="8">
         <v>15</v>
       </c>
-      <c r="U1" s="8">
+      <c r="W1" s="8">
         <v>16</v>
       </c>
-      <c r="V1" s="8">
+      <c r="X1" s="8">
         <v>17</v>
       </c>
-      <c r="W1" s="8">
+      <c r="Y1" s="8">
         <v>18</v>
       </c>
-      <c r="X1" s="8">
+      <c r="Z1" s="8">
         <v>19</v>
       </c>
-      <c r="Y1" s="8">
+      <c r="AA1" s="8">
         <v>20</v>
       </c>
-      <c r="Z1" s="8">
+      <c r="AB1" s="8">
         <v>21</v>
       </c>
-      <c r="AA1" s="8">
+      <c r="AC1" s="8">
         <v>22</v>
       </c>
-      <c r="AB1" s="8">
+      <c r="AD1" s="8">
         <v>23</v>
       </c>
-      <c r="AC1" s="8">
+      <c r="AE1" s="8">
         <v>24</v>
       </c>
-      <c r="AD1" s="8">
+      <c r="AF1" s="8">
         <v>25</v>
       </c>
-      <c r="AE1" s="8">
+      <c r="AG1" s="8">
         <v>26</v>
       </c>
-      <c r="AF1" s="8">
+      <c r="AH1" s="8">
         <v>27</v>
       </c>
-      <c r="AG1" s="8">
+      <c r="AI1" s="8">
         <v>28</v>
       </c>
-      <c r="AH1" s="8">
+      <c r="AJ1" s="8">
         <v>29</v>
       </c>
-      <c r="AI1" s="8">
+      <c r="AK1" s="8">
         <v>30</v>
       </c>
-      <c r="AJ1" s="8">
+      <c r="AL1" s="8">
         <v>31</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AN1" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="AM1" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="AMG1"/>
-      <c r="AMH1"/>
       <c r="AMI1"/>
       <c r="AMJ1"/>
-    </row>
-    <row r="2" spans="1:1024" x14ac:dyDescent="0.2">
+      <c r="AMK1"/>
+      <c r="AML1"/>
+    </row>
+    <row r="2" spans="1:1026" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1410,22 +1427,24 @@
       <c r="C2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D2"/>
-      <c r="E2">
-        <f t="shared" ref="E2:E29" si="0">31-COUNTIF(F2:AJ2,8)</f>
+      <c r="D2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G2">
+        <f>31-COUNTIF(H2:AL2,8)</f>
         <v>12</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" s="7">
-        <v>8</v>
-      </c>
-      <c r="I2" s="7">
-        <v>8</v>
+      <c r="H2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="J2" s="7">
         <v>8</v>
@@ -1433,29 +1452,29 @@
       <c r="K2" s="7">
         <v>8</v>
       </c>
-      <c r="L2" s="7" t="s">
-        <v>197</v>
+      <c r="L2" s="7">
+        <v>8</v>
       </c>
       <c r="M2" s="7">
         <v>8</v>
       </c>
-      <c r="N2" s="7">
-        <v>8</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>92</v>
+      <c r="N2" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="O2" s="7">
+        <v>8</v>
+      </c>
+      <c r="P2" s="7">
+        <v>8</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="R2" s="7">
-        <v>8</v>
-      </c>
-      <c r="S2" s="7">
-        <v>8</v>
+        <v>91</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="T2" s="7">
         <v>8</v>
@@ -1475,29 +1494,29 @@
       <c r="Y2" s="7">
         <v>8</v>
       </c>
-      <c r="Z2" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA2" s="7" t="s">
-        <v>56</v>
+      <c r="Z2" s="7">
+        <v>8</v>
+      </c>
+      <c r="AA2" s="7">
+        <v>8</v>
       </c>
       <c r="AB2" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AC2" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AD2" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AE2" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF2" s="7">
-        <v>8</v>
-      </c>
-      <c r="AG2" s="7">
-        <v>8</v>
+        <v>55</v>
+      </c>
+      <c r="AF2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG2" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="AH2" s="7">
         <v>8</v>
@@ -1509,16 +1528,22 @@
         <v>8</v>
       </c>
       <c r="AK2" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL2" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM2" s="7">
         <v>100</v>
       </c>
-      <c r="AL2" s="6">
+      <c r="AN2" s="6">
         <v>0</v>
       </c>
-      <c r="AM2" s="6">
+      <c r="AO2" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1026" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1528,25 +1553,27 @@
       <c r="C3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D3"/>
-      <c r="E3">
-        <f t="shared" si="0"/>
+      <c r="D3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G3">
+        <f>31-COUNTIF(H3:AL3,8)</f>
         <v>12</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>92</v>
-      </c>
       <c r="H3" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I3" s="7">
-        <v>8</v>
-      </c>
-      <c r="J3" s="7">
-        <v>8</v>
+        <v>91</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="K3" s="7">
         <v>8</v>
@@ -1560,32 +1587,32 @@
       <c r="N3" s="7">
         <v>8</v>
       </c>
-      <c r="O3" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>70</v>
+      <c r="O3" s="7">
+        <v>8</v>
+      </c>
+      <c r="P3" s="7">
+        <v>8</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="U3" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="V3" s="7">
-        <v>8</v>
-      </c>
-      <c r="W3" s="7">
-        <v>8</v>
+        <v>69</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="X3" s="7">
         <v>8</v>
@@ -1599,17 +1626,17 @@
       <c r="AA3" s="7">
         <v>8</v>
       </c>
-      <c r="AB3" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="AC3" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="AD3" s="7">
-        <v>8</v>
-      </c>
-      <c r="AE3" s="7">
-        <v>8</v>
+      <c r="AB3" s="7">
+        <v>8</v>
+      </c>
+      <c r="AC3" s="7">
+        <v>8</v>
+      </c>
+      <c r="AD3" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="AE3" s="7" t="s">
+        <v>197</v>
       </c>
       <c r="AF3" s="7">
         <v>8</v>
@@ -1627,16 +1654,22 @@
         <v>8</v>
       </c>
       <c r="AK3" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL3" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM3" s="7">
         <v>100</v>
       </c>
-      <c r="AL3" s="6">
+      <c r="AN3" s="6">
         <v>0</v>
       </c>
-      <c r="AM3" s="6">
+      <c r="AO3" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1026" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1644,19 +1677,21 @@
         <v>36</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4"/>
-      <c r="E4">
-        <f t="shared" si="0"/>
+        <v>198</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G4">
+        <f>31-COUNTIF(H4:AL4,8)</f>
         <v>0</v>
       </c>
-      <c r="F4" s="7">
-        <v>8</v>
-      </c>
-      <c r="G4" s="7">
-        <v>8</v>
-      </c>
       <c r="H4" s="7">
         <v>8</v>
       </c>
@@ -1745,36 +1780,44 @@
         <v>8</v>
       </c>
       <c r="AK4" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL4" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM4" s="7">
         <v>100</v>
       </c>
-      <c r="AL4" s="6">
+      <c r="AN4" s="6">
         <v>0</v>
       </c>
-      <c r="AM4" s="6">
+      <c r="AO4" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1026" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5"/>
-      <c r="E5">
-        <f t="shared" si="0"/>
+      <c r="D5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G5">
+        <f>31-COUNTIF(H5:AL5,8)</f>
         <v>0</v>
       </c>
-      <c r="F5" s="7">
-        <v>8</v>
-      </c>
-      <c r="G5" s="7">
-        <v>8</v>
-      </c>
       <c r="H5" s="7">
         <v>8</v>
       </c>
@@ -1863,36 +1906,44 @@
         <v>8</v>
       </c>
       <c r="AK5" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL5" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM5" s="7">
         <v>100</v>
       </c>
-      <c r="AL5" s="6">
+      <c r="AN5" s="6">
         <v>0</v>
       </c>
-      <c r="AM5" s="6">
+      <c r="AO5" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1026" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6"/>
-      <c r="E6">
-        <f t="shared" si="0"/>
+      <c r="D6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G6">
+        <f>31-COUNTIF(H6:AL6,8)</f>
         <v>0</v>
       </c>
-      <c r="F6" s="7">
-        <v>8</v>
-      </c>
-      <c r="G6" s="7">
-        <v>8</v>
-      </c>
       <c r="H6" s="7">
         <v>8</v>
       </c>
@@ -1981,36 +2032,44 @@
         <v>8</v>
       </c>
       <c r="AK6" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL6" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM6" s="7">
         <v>100</v>
       </c>
-      <c r="AL6" s="6">
+      <c r="AN6" s="6">
         <v>0</v>
       </c>
-      <c r="AM6" s="6">
+      <c r="AO6" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1026" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7"/>
-      <c r="E7">
-        <f t="shared" si="0"/>
+      <c r="D7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G7">
+        <f>31-COUNTIF(H7:AL7,8)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="7">
-        <v>8</v>
-      </c>
-      <c r="G7" s="7">
-        <v>8</v>
-      </c>
       <c r="H7" s="7">
         <v>8</v>
       </c>
@@ -2099,272 +2158,296 @@
         <v>8</v>
       </c>
       <c r="AK7" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL7" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM7" s="7">
         <v>100</v>
       </c>
-      <c r="AL7" s="6">
+      <c r="AN7" s="6">
         <v>0</v>
       </c>
-      <c r="AM7" s="6">
+      <c r="AO7" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1026" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="D8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G8">
+        <f>31-COUNTIF(H8:AL8,8)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="7">
+        <v>8</v>
+      </c>
+      <c r="I8" s="7">
+        <v>8</v>
+      </c>
+      <c r="J8" s="7">
+        <v>8</v>
+      </c>
+      <c r="K8" s="7">
+        <v>8</v>
+      </c>
+      <c r="L8" s="7">
+        <v>8</v>
+      </c>
+      <c r="M8" s="7">
+        <v>8</v>
+      </c>
+      <c r="N8" s="7">
+        <v>8</v>
+      </c>
+      <c r="O8" s="7">
+        <v>8</v>
+      </c>
+      <c r="P8" s="7">
+        <v>8</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>8</v>
+      </c>
+      <c r="R8" s="7">
+        <v>8</v>
+      </c>
+      <c r="S8" s="7">
+        <v>8</v>
+      </c>
+      <c r="T8" s="7">
+        <v>8</v>
+      </c>
+      <c r="U8" s="7">
+        <v>8</v>
+      </c>
+      <c r="V8" s="7">
+        <v>8</v>
+      </c>
+      <c r="W8" s="7">
+        <v>8</v>
+      </c>
+      <c r="X8" s="7">
+        <v>8</v>
+      </c>
+      <c r="Y8" s="7">
+        <v>8</v>
+      </c>
+      <c r="Z8" s="7">
+        <v>8</v>
+      </c>
+      <c r="AA8" s="7">
+        <v>8</v>
+      </c>
+      <c r="AB8" s="7">
+        <v>8</v>
+      </c>
+      <c r="AC8" s="7">
+        <v>8</v>
+      </c>
+      <c r="AD8" s="7">
+        <v>8</v>
+      </c>
+      <c r="AE8" s="7">
+        <v>8</v>
+      </c>
+      <c r="AF8" s="7">
+        <v>8</v>
+      </c>
+      <c r="AG8" s="7">
+        <v>8</v>
+      </c>
+      <c r="AH8" s="7">
+        <v>8</v>
+      </c>
+      <c r="AI8" s="7">
+        <v>8</v>
+      </c>
+      <c r="AJ8" s="7">
+        <v>8</v>
+      </c>
+      <c r="AK8" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL8" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM8" s="7">
+        <v>100</v>
+      </c>
+      <c r="AN8" s="6">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1026" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D8"/>
-      <c r="E8">
-        <f t="shared" si="0"/>
+      <c r="C9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G9">
+        <f>31-COUNTIF(H9:AL9,8)</f>
         <v>0</v>
       </c>
-      <c r="F8" s="7">
-        <v>8</v>
-      </c>
-      <c r="G8" s="7">
-        <v>8</v>
-      </c>
-      <c r="H8" s="7">
-        <v>8</v>
-      </c>
-      <c r="I8" s="7">
-        <v>8</v>
-      </c>
-      <c r="J8" s="7">
-        <v>8</v>
-      </c>
-      <c r="K8" s="7">
-        <v>8</v>
-      </c>
-      <c r="L8" s="7">
-        <v>8</v>
-      </c>
-      <c r="M8" s="7">
-        <v>8</v>
-      </c>
-      <c r="N8" s="7">
-        <v>8</v>
-      </c>
-      <c r="O8" s="7">
-        <v>8</v>
-      </c>
-      <c r="P8" s="7">
-        <v>8</v>
-      </c>
-      <c r="Q8" s="7">
-        <v>8</v>
-      </c>
-      <c r="R8" s="7">
-        <v>8</v>
-      </c>
-      <c r="S8" s="7">
-        <v>8</v>
-      </c>
-      <c r="T8" s="7">
-        <v>8</v>
-      </c>
-      <c r="U8" s="7">
-        <v>8</v>
-      </c>
-      <c r="V8" s="7">
-        <v>8</v>
-      </c>
-      <c r="W8" s="7">
-        <v>8</v>
-      </c>
-      <c r="X8" s="7">
-        <v>8</v>
-      </c>
-      <c r="Y8" s="7">
-        <v>8</v>
-      </c>
-      <c r="Z8" s="7">
-        <v>8</v>
-      </c>
-      <c r="AA8" s="7">
-        <v>8</v>
-      </c>
-      <c r="AB8" s="7">
-        <v>8</v>
-      </c>
-      <c r="AC8" s="7">
-        <v>8</v>
-      </c>
-      <c r="AD8" s="7">
-        <v>8</v>
-      </c>
-      <c r="AE8" s="7">
-        <v>8</v>
-      </c>
-      <c r="AF8" s="7">
-        <v>8</v>
-      </c>
-      <c r="AG8" s="7">
-        <v>8</v>
-      </c>
-      <c r="AH8" s="7">
-        <v>8</v>
-      </c>
-      <c r="AI8" s="7">
-        <v>8</v>
-      </c>
-      <c r="AJ8" s="7">
-        <v>8</v>
-      </c>
-      <c r="AK8" s="7">
+      <c r="H9" s="7">
+        <v>8</v>
+      </c>
+      <c r="I9" s="7">
+        <v>8</v>
+      </c>
+      <c r="J9" s="7">
+        <v>8</v>
+      </c>
+      <c r="K9" s="7">
+        <v>8</v>
+      </c>
+      <c r="L9" s="7">
+        <v>8</v>
+      </c>
+      <c r="M9" s="7">
+        <v>8</v>
+      </c>
+      <c r="N9" s="7">
+        <v>8</v>
+      </c>
+      <c r="O9" s="7">
+        <v>8</v>
+      </c>
+      <c r="P9" s="7">
+        <v>8</v>
+      </c>
+      <c r="Q9" s="7">
+        <v>8</v>
+      </c>
+      <c r="R9" s="7">
+        <v>8</v>
+      </c>
+      <c r="S9" s="7">
+        <v>8</v>
+      </c>
+      <c r="T9" s="7">
+        <v>8</v>
+      </c>
+      <c r="U9" s="7">
+        <v>8</v>
+      </c>
+      <c r="V9" s="7">
+        <v>8</v>
+      </c>
+      <c r="W9" s="7">
+        <v>8</v>
+      </c>
+      <c r="X9" s="7">
+        <v>8</v>
+      </c>
+      <c r="Y9" s="7">
+        <v>8</v>
+      </c>
+      <c r="Z9" s="7">
+        <v>8</v>
+      </c>
+      <c r="AA9" s="7">
+        <v>8</v>
+      </c>
+      <c r="AB9" s="7">
+        <v>8</v>
+      </c>
+      <c r="AC9" s="7">
+        <v>8</v>
+      </c>
+      <c r="AD9" s="7">
+        <v>8</v>
+      </c>
+      <c r="AE9" s="7">
+        <v>8</v>
+      </c>
+      <c r="AF9" s="7">
+        <v>8</v>
+      </c>
+      <c r="AG9" s="7">
+        <v>8</v>
+      </c>
+      <c r="AH9" s="7">
+        <v>8</v>
+      </c>
+      <c r="AI9" s="7">
+        <v>8</v>
+      </c>
+      <c r="AJ9" s="7">
+        <v>8</v>
+      </c>
+      <c r="AK9" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL9" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM9" s="7">
         <v>100</v>
       </c>
-      <c r="AL8" s="6">
+      <c r="AN9" s="6">
         <v>0</v>
       </c>
-      <c r="AM8" s="6">
+      <c r="AO9" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9"/>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="7">
-        <v>8</v>
-      </c>
-      <c r="G9" s="7">
-        <v>8</v>
-      </c>
-      <c r="H9" s="7">
-        <v>8</v>
-      </c>
-      <c r="I9" s="7">
-        <v>8</v>
-      </c>
-      <c r="J9" s="7">
-        <v>8</v>
-      </c>
-      <c r="K9" s="7">
-        <v>8</v>
-      </c>
-      <c r="L9" s="7">
-        <v>8</v>
-      </c>
-      <c r="M9" s="7">
-        <v>8</v>
-      </c>
-      <c r="N9" s="7">
-        <v>8</v>
-      </c>
-      <c r="O9" s="7">
-        <v>8</v>
-      </c>
-      <c r="P9" s="7">
-        <v>8</v>
-      </c>
-      <c r="Q9" s="7">
-        <v>8</v>
-      </c>
-      <c r="R9" s="7">
-        <v>8</v>
-      </c>
-      <c r="S9" s="7">
-        <v>8</v>
-      </c>
-      <c r="T9" s="7">
-        <v>8</v>
-      </c>
-      <c r="U9" s="7">
-        <v>8</v>
-      </c>
-      <c r="V9" s="7">
-        <v>8</v>
-      </c>
-      <c r="W9" s="7">
-        <v>8</v>
-      </c>
-      <c r="X9" s="7">
-        <v>8</v>
-      </c>
-      <c r="Y9" s="7">
-        <v>8</v>
-      </c>
-      <c r="Z9" s="7">
-        <v>8</v>
-      </c>
-      <c r="AA9" s="7">
-        <v>8</v>
-      </c>
-      <c r="AB9" s="7">
-        <v>8</v>
-      </c>
-      <c r="AC9" s="7">
-        <v>8</v>
-      </c>
-      <c r="AD9" s="7">
-        <v>8</v>
-      </c>
-      <c r="AE9" s="7">
-        <v>8</v>
-      </c>
-      <c r="AF9" s="7">
-        <v>8</v>
-      </c>
-      <c r="AG9" s="7">
-        <v>8</v>
-      </c>
-      <c r="AH9" s="7">
-        <v>8</v>
-      </c>
-      <c r="AI9" s="7">
-        <v>8</v>
-      </c>
-      <c r="AJ9" s="7">
-        <v>8</v>
-      </c>
-      <c r="AK9" s="7">
-        <v>100</v>
-      </c>
-      <c r="AL9" s="6">
-        <v>0</v>
-      </c>
-      <c r="AM9" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1026" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10"/>
-      <c r="E10">
-        <f t="shared" si="0"/>
+      <c r="D10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G10">
+        <f>31-COUNTIF(H10:AL10,8)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="7">
-        <v>8</v>
-      </c>
-      <c r="G10" s="7">
-        <v>8</v>
-      </c>
       <c r="H10" s="7">
         <v>8</v>
       </c>
@@ -2453,36 +2536,44 @@
         <v>8</v>
       </c>
       <c r="AK10" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL10" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM10" s="7">
         <v>100</v>
       </c>
-      <c r="AL10" s="6">
+      <c r="AN10" s="6">
         <v>0</v>
       </c>
-      <c r="AM10" s="6">
+      <c r="AO10" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1026" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11"/>
-      <c r="E11">
-        <f t="shared" si="0"/>
+      <c r="D11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G11">
+        <f>31-COUNTIF(H11:AL11,8)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="7">
-        <v>8</v>
-      </c>
-      <c r="G11" s="7">
-        <v>8</v>
-      </c>
       <c r="H11" s="7">
         <v>8</v>
       </c>
@@ -2571,36 +2662,44 @@
         <v>8</v>
       </c>
       <c r="AK11" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL11" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM11" s="7">
         <v>100</v>
       </c>
-      <c r="AL11" s="6">
+      <c r="AN11" s="6">
         <v>0</v>
       </c>
-      <c r="AM11" s="6">
+      <c r="AO11" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1026" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12"/>
-      <c r="E12">
-        <f t="shared" si="0"/>
+      <c r="D12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G12">
+        <f>31-COUNTIF(H12:AL12,8)</f>
         <v>0</v>
       </c>
-      <c r="F12" s="7">
-        <v>8</v>
-      </c>
-      <c r="G12" s="7">
-        <v>8</v>
-      </c>
       <c r="H12" s="7">
         <v>8</v>
       </c>
@@ -2689,63 +2788,71 @@
         <v>8</v>
       </c>
       <c r="AK12" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL12" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM12" s="7">
         <v>100</v>
       </c>
-      <c r="AL12" s="6">
+      <c r="AN12" s="6">
         <v>0</v>
       </c>
-      <c r="AM12" s="6">
+      <c r="AO12" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1026" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="D13" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G13">
+        <f>31-COUNTIF(H13:AL13,8)</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="7">
+        <v>8</v>
+      </c>
+      <c r="I13" s="7">
+        <v>8</v>
+      </c>
+      <c r="J13" s="7">
+        <v>8</v>
+      </c>
+      <c r="K13" s="7">
+        <v>8</v>
+      </c>
+      <c r="L13" s="7">
+        <v>8</v>
+      </c>
+      <c r="M13" s="7">
+        <v>8</v>
+      </c>
+      <c r="N13" s="7">
+        <v>8</v>
+      </c>
+      <c r="O13" s="7">
+        <v>8</v>
+      </c>
+      <c r="P13" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D13"/>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F13" s="7">
-        <v>8</v>
-      </c>
-      <c r="G13" s="7">
-        <v>8</v>
-      </c>
-      <c r="H13" s="7">
-        <v>8</v>
-      </c>
-      <c r="I13" s="7">
-        <v>8</v>
-      </c>
-      <c r="J13" s="7">
-        <v>8</v>
-      </c>
-      <c r="K13" s="7">
-        <v>8</v>
-      </c>
-      <c r="L13" s="7">
-        <v>8</v>
-      </c>
-      <c r="M13" s="7">
-        <v>8</v>
-      </c>
-      <c r="N13" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="O13" s="7">
-        <v>8</v>
-      </c>
-      <c r="P13" s="7">
-        <v>8</v>
-      </c>
       <c r="Q13" s="7">
         <v>8</v>
       </c>
@@ -2807,154 +2914,170 @@
         <v>8</v>
       </c>
       <c r="AK13" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL13" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM13" s="7">
         <v>100</v>
       </c>
-      <c r="AL13" s="6">
+      <c r="AN13" s="6">
         <v>0</v>
       </c>
-      <c r="AM13" s="6">
+      <c r="AO13" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1026" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="D14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G14">
+        <f>31-COUNTIF(H14:AL14,8)</f>
+        <v>5</v>
+      </c>
+      <c r="H14" s="7">
+        <v>8</v>
+      </c>
+      <c r="I14" s="7">
+        <v>8</v>
+      </c>
+      <c r="J14" s="7">
+        <v>8</v>
+      </c>
+      <c r="K14" s="7">
+        <v>8</v>
+      </c>
+      <c r="L14" s="7">
+        <v>8</v>
+      </c>
+      <c r="M14" s="7">
+        <v>8</v>
+      </c>
+      <c r="N14" s="7">
+        <v>8</v>
+      </c>
+      <c r="O14" s="7">
+        <v>8</v>
+      </c>
+      <c r="P14" s="7">
+        <v>8</v>
+      </c>
+      <c r="Q14" s="7">
+        <v>8</v>
+      </c>
+      <c r="R14" s="7">
+        <v>8</v>
+      </c>
+      <c r="S14" s="7">
+        <v>8</v>
+      </c>
+      <c r="T14" s="7">
+        <v>8</v>
+      </c>
+      <c r="U14" s="7">
+        <v>8</v>
+      </c>
+      <c r="V14" s="7">
+        <v>8</v>
+      </c>
+      <c r="W14" s="7">
+        <v>8</v>
+      </c>
+      <c r="X14" s="7">
+        <v>8</v>
+      </c>
+      <c r="Y14" s="7">
+        <v>8</v>
+      </c>
+      <c r="Z14" s="7">
+        <v>8</v>
+      </c>
+      <c r="AA14" s="7">
+        <v>8</v>
+      </c>
+      <c r="AB14" s="7">
+        <v>8</v>
+      </c>
+      <c r="AC14" s="7">
+        <v>8</v>
+      </c>
+      <c r="AD14" s="7">
+        <v>8</v>
+      </c>
+      <c r="AE14" s="7">
+        <v>8</v>
+      </c>
+      <c r="AF14" s="7">
+        <v>8</v>
+      </c>
+      <c r="AG14" s="7">
+        <v>8</v>
+      </c>
+      <c r="AH14" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D14"/>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="F14" s="7">
-        <v>8</v>
-      </c>
-      <c r="G14" s="7">
-        <v>8</v>
-      </c>
-      <c r="H14" s="7">
-        <v>8</v>
-      </c>
-      <c r="I14" s="7">
-        <v>8</v>
-      </c>
-      <c r="J14" s="7">
-        <v>8</v>
-      </c>
-      <c r="K14" s="7">
-        <v>8</v>
-      </c>
-      <c r="L14" s="7">
-        <v>8</v>
-      </c>
-      <c r="M14" s="7">
-        <v>8</v>
-      </c>
-      <c r="N14" s="7">
-        <v>8</v>
-      </c>
-      <c r="O14" s="7">
-        <v>8</v>
-      </c>
-      <c r="P14" s="7">
-        <v>8</v>
-      </c>
-      <c r="Q14" s="7">
-        <v>8</v>
-      </c>
-      <c r="R14" s="7">
-        <v>8</v>
-      </c>
-      <c r="S14" s="7">
-        <v>8</v>
-      </c>
-      <c r="T14" s="7">
-        <v>8</v>
-      </c>
-      <c r="U14" s="7">
-        <v>8</v>
-      </c>
-      <c r="V14" s="7">
-        <v>8</v>
-      </c>
-      <c r="W14" s="7">
-        <v>8</v>
-      </c>
-      <c r="X14" s="7">
-        <v>8</v>
-      </c>
-      <c r="Y14" s="7">
-        <v>8</v>
-      </c>
-      <c r="Z14" s="7">
-        <v>8</v>
-      </c>
-      <c r="AA14" s="7">
-        <v>8</v>
-      </c>
-      <c r="AB14" s="7">
-        <v>8</v>
-      </c>
-      <c r="AC14" s="7">
-        <v>8</v>
-      </c>
-      <c r="AD14" s="7">
-        <v>8</v>
-      </c>
-      <c r="AE14" s="7">
-        <v>8</v>
-      </c>
-      <c r="AF14" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG14" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH14" s="7" t="s">
-        <v>59</v>
-      </c>
       <c r="AI14" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ14" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK14" s="7">
+        <v>58</v>
+      </c>
+      <c r="AK14" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL14" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM14" s="7">
         <v>100</v>
       </c>
-      <c r="AL14" s="6">
+      <c r="AN14" s="6">
         <v>0</v>
       </c>
-      <c r="AM14" s="6">
+      <c r="AO14" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1026" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15"/>
-      <c r="E15">
-        <f t="shared" si="0"/>
+      <c r="D15" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G15">
+        <f>31-COUNTIF(H15:AL15,8)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="7">
-        <v>8</v>
-      </c>
-      <c r="G15" s="7">
-        <v>8</v>
-      </c>
       <c r="H15" s="7">
         <v>8</v>
       </c>
@@ -3043,36 +3166,44 @@
         <v>8</v>
       </c>
       <c r="AK15" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL15" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM15" s="7">
         <v>100</v>
       </c>
-      <c r="AL15" s="6">
+      <c r="AN15" s="6">
         <v>0</v>
       </c>
-      <c r="AM15" s="6">
+      <c r="AO15" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:1024" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1026" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16"/>
-      <c r="E16">
-        <f t="shared" si="0"/>
+      <c r="D16" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G16">
+        <f>31-COUNTIF(H16:AL16,8)</f>
         <v>0</v>
       </c>
-      <c r="F16" s="7">
-        <v>8</v>
-      </c>
-      <c r="G16" s="7">
-        <v>8</v>
-      </c>
       <c r="H16" s="7">
         <v>8</v>
       </c>
@@ -3161,36 +3292,44 @@
         <v>8</v>
       </c>
       <c r="AK16" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL16" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM16" s="7">
         <v>100</v>
       </c>
-      <c r="AL16" s="6">
+      <c r="AN16" s="6">
         <v>0</v>
       </c>
-      <c r="AM16" s="6">
+      <c r="AO16" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17"/>
-      <c r="E17">
-        <f t="shared" si="0"/>
+      <c r="D17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G17">
+        <f>31-COUNTIF(H17:AL17,8)</f>
         <v>0</v>
       </c>
-      <c r="F17" s="7">
-        <v>8</v>
-      </c>
-      <c r="G17" s="7">
-        <v>8</v>
-      </c>
       <c r="H17" s="7">
         <v>8</v>
       </c>
@@ -3279,36 +3418,44 @@
         <v>8</v>
       </c>
       <c r="AK17" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL17" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM17" s="7">
         <v>100</v>
       </c>
-      <c r="AL17" s="6">
+      <c r="AN17" s="6">
         <v>0</v>
       </c>
-      <c r="AM17" s="6">
+      <c r="AO17" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18"/>
-      <c r="E18">
-        <f t="shared" si="0"/>
+      <c r="D18" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G18">
+        <f>31-COUNTIF(H18:AL18,8)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="7">
-        <v>8</v>
-      </c>
-      <c r="G18" s="7">
-        <v>8</v>
-      </c>
       <c r="H18" s="7">
         <v>8</v>
       </c>
@@ -3397,101 +3544,109 @@
         <v>8</v>
       </c>
       <c r="AK18" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL18" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM18" s="7">
         <v>100</v>
       </c>
-      <c r="AL18" s="6">
+      <c r="AN18" s="6">
         <v>0</v>
       </c>
-      <c r="AM18" s="6">
+      <c r="AO18" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="D19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G19">
+        <f>31-COUNTIF(H19:AL19,8)</f>
+        <v>12</v>
+      </c>
+      <c r="H19" s="7">
+        <v>8</v>
+      </c>
+      <c r="I19" s="7">
+        <v>8</v>
+      </c>
+      <c r="J19" s="7">
+        <v>8</v>
+      </c>
+      <c r="K19" s="7">
+        <v>8</v>
+      </c>
+      <c r="L19" s="7">
+        <v>8</v>
+      </c>
+      <c r="M19" s="7">
+        <v>8</v>
+      </c>
+      <c r="N19" s="7">
+        <v>8</v>
+      </c>
+      <c r="O19" s="7">
+        <v>8</v>
+      </c>
+      <c r="P19" s="7">
+        <v>8</v>
+      </c>
+      <c r="Q19" s="7">
+        <v>8</v>
+      </c>
+      <c r="R19" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D19"/>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="F19" s="7">
-        <v>8</v>
-      </c>
-      <c r="G19" s="7">
-        <v>8</v>
-      </c>
-      <c r="H19" s="7">
-        <v>8</v>
-      </c>
-      <c r="I19" s="7">
-        <v>8</v>
-      </c>
-      <c r="J19" s="7">
-        <v>8</v>
-      </c>
-      <c r="K19" s="7">
-        <v>8</v>
-      </c>
-      <c r="L19" s="7">
-        <v>8</v>
-      </c>
-      <c r="M19" s="7">
-        <v>8</v>
-      </c>
-      <c r="N19" s="7">
-        <v>8</v>
-      </c>
-      <c r="O19" s="7">
-        <v>8</v>
-      </c>
-      <c r="P19" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q19" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="R19" s="7" t="s">
-        <v>70</v>
-      </c>
       <c r="S19" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T19" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="U19" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V19" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W19" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X19" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Y19" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Z19" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AA19" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB19" s="7">
-        <v>8</v>
-      </c>
-      <c r="AC19" s="7">
-        <v>8</v>
+        <v>69</v>
+      </c>
+      <c r="AB19" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC19" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="AD19" s="7">
         <v>8</v>
@@ -3515,36 +3670,44 @@
         <v>8</v>
       </c>
       <c r="AK19" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL19" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM19" s="7">
         <v>50</v>
       </c>
-      <c r="AL19" s="6">
+      <c r="AN19" s="6">
         <v>30</v>
       </c>
-      <c r="AM19" s="6">
+      <c r="AO19" s="6">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20"/>
-      <c r="E20">
-        <f t="shared" si="0"/>
+      <c r="D20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G20">
+        <f>31-COUNTIF(H20:AL20,8)</f>
         <v>0</v>
       </c>
-      <c r="F20" s="7">
-        <v>8</v>
-      </c>
-      <c r="G20" s="7">
-        <v>8</v>
-      </c>
       <c r="H20" s="7">
         <v>8</v>
       </c>
@@ -3633,36 +3796,44 @@
         <v>8</v>
       </c>
       <c r="AK20" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL20" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM20" s="7">
         <v>50</v>
       </c>
-      <c r="AL20" s="6">
+      <c r="AN20" s="6">
         <v>30</v>
       </c>
-      <c r="AM20" s="6">
+      <c r="AO20" s="6">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21"/>
-      <c r="E21">
-        <f t="shared" si="0"/>
+      <c r="D21" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G21">
+        <f>31-COUNTIF(H21:AL21,8)</f>
         <v>0</v>
       </c>
-      <c r="F21" s="7">
-        <v>8</v>
-      </c>
-      <c r="G21" s="7">
-        <v>8</v>
-      </c>
       <c r="H21" s="7">
         <v>8</v>
       </c>
@@ -3751,38 +3922,44 @@
         <v>8</v>
       </c>
       <c r="AK21" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL21" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM21" s="7">
         <v>50</v>
       </c>
-      <c r="AL21" s="6">
+      <c r="AN21" s="6">
         <v>30</v>
       </c>
-      <c r="AM21" s="6">
+      <c r="AO21" s="6">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
+      <c r="F22" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G22">
+        <f>31-COUNTIF(H22:AL22,8)</f>
         <v>0</v>
       </c>
-      <c r="F22" s="7">
-        <v>8</v>
-      </c>
-      <c r="G22" s="7">
-        <v>8</v>
-      </c>
       <c r="H22" s="7">
         <v>8</v>
       </c>
@@ -3871,94 +4048,100 @@
         <v>8</v>
       </c>
       <c r="AK22" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL22" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM22" s="7">
         <v>50</v>
       </c>
-      <c r="AL22" s="6">
+      <c r="AN22" s="6">
         <v>30</v>
       </c>
-      <c r="AM22" s="6">
+      <c r="AO22" s="6">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="D23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G23">
+        <f>31-COUNTIF(H23:AL23,8)</f>
+        <v>13</v>
+      </c>
+      <c r="H23" s="7">
+        <v>8</v>
+      </c>
+      <c r="I23" s="7">
+        <v>8</v>
+      </c>
+      <c r="J23" s="7">
+        <v>8</v>
+      </c>
+      <c r="K23" s="7">
+        <v>8</v>
+      </c>
+      <c r="L23" s="7">
+        <v>8</v>
+      </c>
+      <c r="M23" s="7">
+        <v>8</v>
+      </c>
+      <c r="N23" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="F23" s="7">
-        <v>8</v>
-      </c>
-      <c r="G23" s="7">
-        <v>8</v>
-      </c>
-      <c r="H23" s="7">
-        <v>8</v>
-      </c>
-      <c r="I23" s="7">
-        <v>8</v>
-      </c>
-      <c r="J23" s="7">
-        <v>8</v>
-      </c>
-      <c r="K23" s="7">
-        <v>8</v>
-      </c>
-      <c r="L23" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="M23" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="N23" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="O23" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P23" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q23" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R23" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="S23" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="T23" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="U23" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="V23" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="W23" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="X23" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="Y23" s="7">
-        <v>8</v>
-      </c>
-      <c r="Z23" s="7">
-        <v>8</v>
+        <v>78</v>
+      </c>
+      <c r="Y23" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z23" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="AA23" s="7">
         <v>8</v>
@@ -3991,52 +4174,58 @@
         <v>8</v>
       </c>
       <c r="AK23" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL23" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM23" s="7">
         <v>50</v>
       </c>
-      <c r="AL23" s="6">
+      <c r="AN23" s="6">
         <v>30</v>
       </c>
-      <c r="AM23" s="6">
+      <c r="AO23" s="6">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
+      <c r="F24" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G24">
+        <f>31-COUNTIF(H24:AL24,8)</f>
         <v>5</v>
       </c>
-      <c r="F24" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>59</v>
-      </c>
       <c r="H24" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="K24" s="7">
-        <v>8</v>
-      </c>
-      <c r="L24" s="7">
-        <v>8</v>
+        <v>58</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L24" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="M24" s="7">
         <v>8</v>
@@ -4111,38 +4300,44 @@
         <v>8</v>
       </c>
       <c r="AK24" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL24" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM24" s="7">
         <v>50</v>
       </c>
-      <c r="AL24" s="6">
+      <c r="AN24" s="6">
         <v>10</v>
       </c>
-      <c r="AM24" s="6">
+      <c r="AO24" s="6">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
+      <c r="F25" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G25">
+        <f>31-COUNTIF(H25:AL25,8)</f>
         <v>0</v>
       </c>
-      <c r="F25" s="7">
-        <v>8</v>
-      </c>
-      <c r="G25" s="7">
-        <v>8</v>
-      </c>
       <c r="H25" s="7">
         <v>8</v>
       </c>
@@ -4231,38 +4426,44 @@
         <v>8</v>
       </c>
       <c r="AK25" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL25" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM25" s="7">
         <v>50</v>
       </c>
-      <c r="AL25" s="6">
+      <c r="AN25" s="6">
         <v>10</v>
       </c>
-      <c r="AM25" s="6">
+      <c r="AO25" s="6">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
+      <c r="F26" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G26">
+        <f>31-COUNTIF(H26:AL26,8)</f>
         <v>0</v>
       </c>
-      <c r="F26" s="7">
-        <v>8</v>
-      </c>
-      <c r="G26" s="7">
-        <v>8</v>
-      </c>
       <c r="H26" s="7">
         <v>8</v>
       </c>
@@ -4351,38 +4552,44 @@
         <v>8</v>
       </c>
       <c r="AK26" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL26" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM26" s="7">
         <v>50</v>
       </c>
-      <c r="AL26" s="6">
+      <c r="AN26" s="6">
         <v>20</v>
       </c>
-      <c r="AM26" s="6">
+      <c r="AO26" s="6">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
+      <c r="F27" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G27">
+        <f>31-COUNTIF(H27:AL27,8)</f>
         <v>16</v>
       </c>
-      <c r="F27" s="7">
-        <v>8</v>
-      </c>
-      <c r="G27" s="7">
-        <v>8</v>
-      </c>
       <c r="H27" s="7">
         <v>8</v>
       </c>
@@ -4422,87 +4629,93 @@
       <c r="T27" s="7">
         <v>8</v>
       </c>
-      <c r="U27" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="V27" s="7" t="s">
-        <v>70</v>
+      <c r="U27" s="7">
+        <v>8</v>
+      </c>
+      <c r="V27" s="7">
+        <v>8</v>
       </c>
       <c r="W27" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X27" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Y27" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Z27" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AA27" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AB27" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AC27" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AD27" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AE27" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AF27" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AG27" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AH27" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AI27" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AJ27" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="AK27" s="7">
+        <v>69</v>
+      </c>
+      <c r="AK27" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL27" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM27" s="7">
         <v>0</v>
       </c>
-      <c r="AL27" s="6">
+      <c r="AN27" s="6">
         <v>50</v>
       </c>
-      <c r="AM27" s="6">
+      <c r="AO27" s="6">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E28">
-        <f t="shared" si="0"/>
+      <c r="F28" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G28">
+        <f>31-COUNTIF(H28:AL28,8)</f>
         <v>0</v>
       </c>
-      <c r="F28" s="7">
-        <v>8</v>
-      </c>
-      <c r="G28" s="7">
-        <v>8</v>
-      </c>
       <c r="H28" s="7">
         <v>8</v>
       </c>
@@ -4591,82 +4804,91 @@
         <v>8</v>
       </c>
       <c r="AK28" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL28" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM28" s="7">
         <v>0</v>
       </c>
-      <c r="AL28" s="6">
+      <c r="AN28" s="6">
         <v>50</v>
       </c>
-      <c r="AM28" s="6">
+      <c r="AO28" s="6">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="D29" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G29">
+        <f>31-COUNTIF(H29:AL29,8)</f>
+        <v>11</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="L29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="N29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="O29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="P29" s="7">
+        <v>8</v>
+      </c>
+      <c r="Q29" s="7">
+        <v>8</v>
+      </c>
+      <c r="R29" s="7">
+        <v>8</v>
+      </c>
+      <c r="S29" s="7">
+        <v>8</v>
+      </c>
+      <c r="T29" s="7">
+        <v>8</v>
+      </c>
+      <c r="U29" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="E29">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="J29" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="K29" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="L29" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="M29" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="N29" s="7">
-        <v>8</v>
-      </c>
-      <c r="O29" s="7">
-        <v>8</v>
-      </c>
-      <c r="P29" s="7">
-        <v>8</v>
-      </c>
-      <c r="Q29" s="7">
-        <v>8</v>
-      </c>
-      <c r="R29" s="7">
-        <v>8</v>
-      </c>
-      <c r="S29" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="T29" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="U29" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="V29" s="7">
-        <v>8</v>
-      </c>
-      <c r="W29" s="7">
-        <v>8</v>
+      <c r="V29" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="W29" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="X29" s="7">
         <v>8</v>
@@ -4708,574 +4930,1039 @@
         <v>8</v>
       </c>
       <c r="AK29" s="7">
+        <v>8</v>
+      </c>
+      <c r="AL29" s="7">
+        <v>8</v>
+      </c>
+      <c r="AM29" s="7">
         <v>0</v>
       </c>
-      <c r="AL29" s="6">
+      <c r="AN29" s="6">
         <v>50</v>
       </c>
-      <c r="AM29" s="6">
+      <c r="AO29" s="6">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="D30" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="D31" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="32" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C34" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C37" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C40" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C41" s="9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="C42" s="9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C43" s="9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C44" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="C44" s="9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C45" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C46" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C46" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="C47" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C48" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="C48" s="9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C49" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C50" s="9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C51" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="C51" s="9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C52" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C52" s="9" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C53" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C53" s="9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C54" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="C54" s="9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C55" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="C55" s="9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="C56" s="9" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C57" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="9" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C58" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="C58" s="9" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D58" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C59" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="C59" s="9" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C60" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="C60" s="9" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D60" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C61" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="C61" s="9" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D61" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C62" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C62" s="9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D62" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C63" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="C63" s="9" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D63" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C64" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="C64" s="9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D64" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C65" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="C65" s="9" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D65" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C66" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="C66" s="9" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D66" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C67" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C67" s="9" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D67" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="C68" s="9" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D68" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C69" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C69" s="9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D69" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C70" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="C70" s="9" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D70" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C71" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="C71" s="9" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D71" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C72" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="C72" s="9" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D72" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C73" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="C73" s="9" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D73" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C75" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="C75" s="9" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D75" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C76" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="C76" s="9" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D76" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C77" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="C77" s="9" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D77" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C78" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="C78" s="9" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D78" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C79" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="C79" s="9" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D79" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C80" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="C80" s="9" t="s">
-        <v>193</v>
+      <c r="D80" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified and improve the final files
</commit_message>
<xml_diff>
--- a/Data/TS_2016_data.xlsx
+++ b/Data/TS_2016_data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="200">
   <si>
     <t>Date</t>
   </si>
@@ -198,9 +198,6 @@
     <t>Frank Patrick</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>NDONG eps NGUEMA</t>
   </si>
   <si>
@@ -256,9 +253,6 @@
   </si>
   <si>
     <t>Mohammed</t>
-  </si>
-  <si>
-    <t>M</t>
   </si>
   <si>
     <t>LELL</t>
@@ -1266,10 +1260,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML80"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="1" tabSelected="1" view="pageBreakPreview" topLeftCell="D1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F19"/>
+      <selection pane="bottomLeft" activeCell="N23" sqref="N23:Z23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1299,13 +1293,13 @@
         <v>30</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>31</v>
@@ -1404,13 +1398,13 @@
         <v>31</v>
       </c>
       <c r="AM1" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="AO1" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="AMI1"/>
       <c r="AMJ1"/>
@@ -1434,17 +1428,17 @@
         <v>27</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G2">
-        <f>31-COUNTIF(H2:AL2,8)</f>
+        <f t="shared" ref="G2:G29" si="0">31-COUNTIF(H2:AL2,8)</f>
         <v>12</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J2" s="7">
         <v>8</v>
@@ -1459,7 +1453,7 @@
         <v>8</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="O2" s="7">
         <v>8</v>
@@ -1468,13 +1462,13 @@
         <v>8</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="T2" s="7">
         <v>8</v>
@@ -1560,20 +1554,20 @@
         <v>27</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G3">
-        <f>31-COUNTIF(H3:AL3,8)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K3" s="7">
         <v>8</v>
@@ -1594,25 +1588,25 @@
         <v>8</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="U3" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="V3" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="W3" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="X3" s="7">
         <v>8</v>
@@ -1633,10 +1627,10 @@
         <v>8</v>
       </c>
       <c r="AD3" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AE3" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="AF3" s="7">
         <v>8</v>
@@ -1677,7 +1671,7 @@
         <v>36</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>26</v>
@@ -1686,10 +1680,10 @@
         <v>27</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G4">
-        <f>31-COUNTIF(H4:AL4,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4" s="7">
@@ -1812,10 +1806,10 @@
         <v>27</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G5">
-        <f>31-COUNTIF(H5:AL5,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H5" s="7">
@@ -1938,10 +1932,10 @@
         <v>27</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G6">
-        <f>31-COUNTIF(H6:AL6,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H6" s="7">
@@ -2064,10 +2058,10 @@
         <v>27</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G7">
-        <f>31-COUNTIF(H7:AL7,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H7" s="7">
@@ -2190,10 +2184,10 @@
         <v>27</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G8">
-        <f>31-COUNTIF(H8:AL8,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H8" s="7">
@@ -2316,10 +2310,10 @@
         <v>27</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G9">
-        <f>31-COUNTIF(H9:AL9,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H9" s="7">
@@ -2442,10 +2436,10 @@
         <v>27</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G10">
-        <f>31-COUNTIF(H10:AL10,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H10" s="7">
@@ -2568,10 +2562,10 @@
         <v>27</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G11">
-        <f>31-COUNTIF(H11:AL11,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H11" s="7">
@@ -2694,10 +2688,10 @@
         <v>27</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G12">
-        <f>31-COUNTIF(H12:AL12,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H12" s="7">
@@ -2820,10 +2814,10 @@
         <v>27</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G13">
-        <f>31-COUNTIF(H13:AL13,8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H13" s="7">
@@ -2946,10 +2940,10 @@
         <v>27</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G14">
-        <f>31-COUNTIF(H14:AL14,8)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H14" s="7">
@@ -3031,19 +3025,19 @@
         <v>8</v>
       </c>
       <c r="AH14" s="7" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="AI14" s="7" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="AJ14" s="7" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="AK14" s="7" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="AL14" s="7" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="AM14" s="7">
         <v>100</v>
@@ -3060,10 +3054,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>24</v>
@@ -3072,10 +3066,10 @@
         <v>27</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G15">
-        <f>31-COUNTIF(H15:AL15,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H15" s="7">
@@ -3186,10 +3180,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>61</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>62</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>24</v>
@@ -3198,11 +3192,11 @@
         <v>27</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G16">
-        <f>31-COUNTIF(H16:AL16,8)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="H16" s="7">
         <v>8</v>
@@ -3231,8 +3225,8 @@
       <c r="P16" s="7">
         <v>8</v>
       </c>
-      <c r="Q16" s="7">
-        <v>8</v>
+      <c r="Q16" s="7" t="s">
+        <v>194</v>
       </c>
       <c r="R16" s="7">
         <v>8</v>
@@ -3255,8 +3249,8 @@
       <c r="X16" s="7">
         <v>8</v>
       </c>
-      <c r="Y16" s="7">
-        <v>8</v>
+      <c r="Y16" s="7" t="s">
+        <v>194</v>
       </c>
       <c r="Z16" s="7">
         <v>8</v>
@@ -3276,8 +3270,8 @@
       <c r="AE16" s="7">
         <v>8</v>
       </c>
-      <c r="AF16" s="7">
-        <v>8</v>
+      <c r="AF16" s="7" t="s">
+        <v>194</v>
       </c>
       <c r="AG16" s="7">
         <v>8</v>
@@ -3312,10 +3306,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>24</v>
@@ -3324,10 +3318,10 @@
         <v>27</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G17">
-        <f>31-COUNTIF(H17:AL17,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H17" s="7">
@@ -3438,10 +3432,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>65</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>66</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>24</v>
@@ -3450,10 +3444,10 @@
         <v>27</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G18">
-        <f>31-COUNTIF(H18:AL18,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H18" s="7">
@@ -3564,10 +3558,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>68</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>24</v>
@@ -3576,10 +3570,10 @@
         <v>27</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G19">
-        <f>31-COUNTIF(H19:AL19,8)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="H19" s="7">
@@ -3613,40 +3607,40 @@
         <v>8</v>
       </c>
       <c r="R19" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S19" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T19" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="U19" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="V19" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="W19" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="X19" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Y19" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Z19" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AA19" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB19" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AC19" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AD19" s="7">
         <v>8</v>
@@ -3676,13 +3670,13 @@
         <v>8</v>
       </c>
       <c r="AM19" s="7">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="AN19" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AO19" s="6">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.2">
@@ -3690,10 +3684,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>71</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>24</v>
@@ -3702,10 +3696,10 @@
         <v>27</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G20">
-        <f>31-COUNTIF(H20:AL20,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H20" s="7">
@@ -3802,13 +3796,13 @@
         <v>8</v>
       </c>
       <c r="AM20" s="7">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="AN20" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AO20" s="6">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.2">
@@ -3816,10 +3810,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>73</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>24</v>
@@ -3828,10 +3822,10 @@
         <v>27</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G21">
-        <f>31-COUNTIF(H21:AL21,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H21" s="7">
@@ -3928,13 +3922,13 @@
         <v>8</v>
       </c>
       <c r="AM21" s="7">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="AN21" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AO21" s="6">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.2">
@@ -3942,10 +3936,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>75</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>21</v>
@@ -3954,10 +3948,10 @@
         <v>20</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G22">
-        <f>31-COUNTIF(H22:AL22,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H22" s="7">
@@ -4054,13 +4048,13 @@
         <v>8</v>
       </c>
       <c r="AM22" s="7">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="AN22" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AO22" s="6">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.2">
@@ -4068,10 +4062,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>77</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>21</v>
@@ -4080,10 +4074,10 @@
         <v>27</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G23">
-        <f>31-COUNTIF(H23:AL23,8)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="H23" s="7">
@@ -4105,43 +4099,43 @@
         <v>8</v>
       </c>
       <c r="N23" s="7" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="O23" s="7" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="P23" s="7" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="Q23" s="7" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="R23" s="7" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="S23" s="7" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="T23" s="7" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="U23" s="7" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="V23" s="7" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="W23" s="7" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="X23" s="7" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="Y23" s="7" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="Z23" s="7" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="AA23" s="7">
         <v>8</v>
@@ -4180,13 +4174,13 @@
         <v>8</v>
       </c>
       <c r="AM23" s="7">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="AN23" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="AO23" s="6">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:41" x14ac:dyDescent="0.2">
@@ -4194,10 +4188,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>21</v>
@@ -4206,26 +4200,26 @@
         <v>27</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G24">
-        <f>31-COUNTIF(H24:AL24,8)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="M24" s="7">
         <v>8</v>
@@ -4306,13 +4300,13 @@
         <v>8</v>
       </c>
       <c r="AM24" s="7">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="AN24" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AO24" s="6">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:41" x14ac:dyDescent="0.2">
@@ -4320,10 +4314,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>21</v>
@@ -4332,10 +4326,10 @@
         <v>27</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G25">
-        <f>31-COUNTIF(H25:AL25,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H25" s="7">
@@ -4432,13 +4426,13 @@
         <v>8</v>
       </c>
       <c r="AM25" s="7">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="AN25" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AO25" s="6">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.2">
@@ -4446,10 +4440,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>21</v>
@@ -4458,10 +4452,10 @@
         <v>22</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G26">
-        <f>31-COUNTIF(H26:AL26,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H26" s="7">
@@ -4558,13 +4552,13 @@
         <v>8</v>
       </c>
       <c r="AM26" s="7">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="AN26" s="6">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AO26" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.2">
@@ -4572,10 +4566,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>21</v>
@@ -4584,10 +4578,10 @@
         <v>18</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G27">
-        <f>31-COUNTIF(H27:AL27,8)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="H27" s="7">
@@ -4636,61 +4630,61 @@
         <v>8</v>
       </c>
       <c r="W27" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="X27" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Y27" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Z27" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AA27" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB27" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AC27" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AD27" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AE27" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AF27" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AG27" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AH27" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AI27" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AJ27" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AK27" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AL27" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AM27" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AN27" s="6">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AO27" s="6">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.2">
@@ -4698,10 +4692,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>21</v>
@@ -4710,10 +4704,10 @@
         <v>27</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G28">
-        <f>31-COUNTIF(H28:AL28,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H28" s="7">
@@ -4810,13 +4804,13 @@
         <v>8</v>
       </c>
       <c r="AM28" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AN28" s="6">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AO28" s="6">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.2">
@@ -4824,10 +4818,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>24</v>
@@ -4836,35 +4830,35 @@
         <v>18</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G29">
-        <f>31-COUNTIF(H29:AL29,8)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M29" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N29" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O29" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P29" s="7">
         <v>8</v>
@@ -4882,13 +4876,13 @@
         <v>8</v>
       </c>
       <c r="U29" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="V29" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="W29" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="X29" s="7">
         <v>8</v>
@@ -4936,13 +4930,13 @@
         <v>8</v>
       </c>
       <c r="AM29" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AN29" s="6">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AO29" s="6">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.2">
@@ -4950,10 +4944,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>24</v>
@@ -4962,7 +4956,7 @@
         <v>18</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:41" x14ac:dyDescent="0.2">
@@ -4970,10 +4964,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>24</v>
@@ -4982,7 +4976,7 @@
         <v>18</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:41" x14ac:dyDescent="0.2">
@@ -4990,10 +4984,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>24</v>
@@ -5002,7 +4996,7 @@
         <v>18</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -5010,10 +5004,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>24</v>
@@ -5022,7 +5016,7 @@
         <v>18</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -5030,10 +5024,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>24</v>
@@ -5042,7 +5036,7 @@
         <v>18</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -5050,10 +5044,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>24</v>
@@ -5062,7 +5056,7 @@
         <v>18</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -5070,10 +5064,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>24</v>
@@ -5082,7 +5076,7 @@
         <v>18</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -5090,10 +5084,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>24</v>
@@ -5102,7 +5096,7 @@
         <v>18</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -5110,10 +5104,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D38" s="9" t="s">
         <v>24</v>
@@ -5122,7 +5116,7 @@
         <v>18</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -5130,10 +5124,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>24</v>
@@ -5142,7 +5136,7 @@
         <v>18</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -5150,10 +5144,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>24</v>
@@ -5162,7 +5156,7 @@
         <v>18</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -5170,10 +5164,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>24</v>
@@ -5182,7 +5176,7 @@
         <v>18</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -5190,10 +5184,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D42" s="9" t="s">
         <v>24</v>
@@ -5202,7 +5196,7 @@
         <v>18</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -5210,10 +5204,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D43" s="9" t="s">
         <v>24</v>
@@ -5222,7 +5216,7 @@
         <v>18</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -5230,10 +5224,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D44" s="9" t="s">
         <v>24</v>
@@ -5242,7 +5236,7 @@
         <v>18</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -5250,10 +5244,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>24</v>
@@ -5262,7 +5256,7 @@
         <v>18</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -5270,10 +5264,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>19</v>
@@ -5282,7 +5276,7 @@
         <v>18</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -5290,10 +5284,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>19</v>
@@ -5302,7 +5296,7 @@
         <v>18</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -5310,10 +5304,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D48" s="9" t="s">
         <v>19</v>
@@ -5322,7 +5316,7 @@
         <v>18</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -5330,10 +5324,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D49" s="9" t="s">
         <v>19</v>
@@ -5342,7 +5336,7 @@
         <v>18</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -5350,10 +5344,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D50" s="9" t="s">
         <v>19</v>
@@ -5362,7 +5356,7 @@
         <v>18</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -5370,10 +5364,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D51" s="9" t="s">
         <v>19</v>
@@ -5382,7 +5376,7 @@
         <v>18</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -5390,10 +5384,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D52" s="9" t="s">
         <v>19</v>
@@ -5402,7 +5396,7 @@
         <v>18</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -5410,10 +5404,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>19</v>
@@ -5422,7 +5416,7 @@
         <v>18</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -5430,10 +5424,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D54" s="9" t="s">
         <v>19</v>
@@ -5442,7 +5436,7 @@
         <v>18</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -5450,10 +5444,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D55" s="9" t="s">
         <v>19</v>
@@ -5462,7 +5456,7 @@
         <v>18</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -5470,10 +5464,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D56" s="9" t="s">
         <v>19</v>
@@ -5482,7 +5476,7 @@
         <v>18</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -5490,10 +5484,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>19</v>
@@ -5502,7 +5496,7 @@
         <v>18</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -5510,10 +5504,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D58" s="9" t="s">
         <v>19</v>
@@ -5522,7 +5516,7 @@
         <v>18</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -5530,10 +5524,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>19</v>
@@ -5542,7 +5536,7 @@
         <v>18</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -5550,10 +5544,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D60" s="9" t="s">
         <v>19</v>
@@ -5562,7 +5556,7 @@
         <v>18</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -5570,10 +5564,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D61" s="9" t="s">
         <v>19</v>
@@ -5582,7 +5576,7 @@
         <v>18</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -5590,10 +5584,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D62" s="9" t="s">
         <v>19</v>
@@ -5602,7 +5596,7 @@
         <v>18</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -5610,10 +5604,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D63" s="9" t="s">
         <v>19</v>
@@ -5622,7 +5616,7 @@
         <v>18</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -5630,10 +5624,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D64" s="9" t="s">
         <v>19</v>
@@ -5642,7 +5636,7 @@
         <v>18</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -5650,10 +5644,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D65" s="9" t="s">
         <v>19</v>
@@ -5662,7 +5656,7 @@
         <v>18</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -5670,10 +5664,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D66" s="9" t="s">
         <v>19</v>
@@ -5682,7 +5676,7 @@
         <v>18</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -5690,10 +5684,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D67" s="9" t="s">
         <v>19</v>
@@ -5702,7 +5696,7 @@
         <v>18</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -5710,10 +5704,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D68" s="9" t="s">
         <v>19</v>
@@ -5722,7 +5716,7 @@
         <v>18</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -5730,10 +5724,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D69" s="9" t="s">
         <v>19</v>
@@ -5742,7 +5736,7 @@
         <v>18</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -5750,10 +5744,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D70" s="9" t="s">
         <v>19</v>
@@ -5762,7 +5756,7 @@
         <v>18</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -5770,10 +5764,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D71" s="9" t="s">
         <v>19</v>
@@ -5782,7 +5776,7 @@
         <v>18</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -5790,10 +5784,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D72" s="9" t="s">
         <v>19</v>
@@ -5802,7 +5796,7 @@
         <v>18</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -5810,10 +5804,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D73" s="9" t="s">
         <v>19</v>
@@ -5822,7 +5816,7 @@
         <v>18</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -5833,7 +5827,7 @@
         <v>41</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D74" s="9" t="s">
         <v>19</v>
@@ -5842,7 +5836,7 @@
         <v>18</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -5850,10 +5844,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D75" s="9" t="s">
         <v>19</v>
@@ -5862,7 +5856,7 @@
         <v>18</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -5870,10 +5864,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D76" s="9" t="s">
         <v>19</v>
@@ -5882,7 +5876,7 @@
         <v>18</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -5890,10 +5884,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D77" s="9" t="s">
         <v>19</v>
@@ -5902,7 +5896,7 @@
         <v>18</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -5910,10 +5904,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D78" s="9" t="s">
         <v>19</v>
@@ -5922,7 +5916,7 @@
         <v>18</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -5930,10 +5924,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D79" s="9" t="s">
         <v>19</v>
@@ -5942,7 +5936,7 @@
         <v>18</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -5950,10 +5944,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D80" s="9" t="s">
         <v>19</v>
@@ -5962,12 +5956,12 @@
         <v>18</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>

</xml_diff>

<commit_message>
Add all columns  for dates 1 to 31
</commit_message>
<xml_diff>
--- a/Data/TS_2016_data.xlsx
+++ b/Data/TS_2016_data.xlsx
@@ -2414,11 +2414,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMH112"/>
+  <dimension ref="A1:AMJ112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AK1" activeCellId="1" sqref="AJ1:AJ1048576 AK1:AK1048576"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AJ1" sqref="AJ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2429,16 +2429,18 @@
     <col min="4" max="4" width="10.28515625" style="6"/>
     <col min="5" max="5" width="8.7109375" style="6"/>
     <col min="6" max="6" width="10.7109375" style="6"/>
-    <col min="7" max="12" width="1.7109375" style="7"/>
+    <col min="7" max="7" width="2" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="1.7109375" style="7"/>
     <col min="13" max="13" width="2.85546875" style="7"/>
     <col min="14" max="15" width="1.7109375" style="7"/>
     <col min="16" max="35" width="2.7109375" style="7"/>
-    <col min="36" max="36" width="8.7109375"/>
-    <col min="37" max="1019" width="10.5703125" style="6"/>
-    <col min="1020" max="1023" width="10.5703125"/>
+    <col min="36" max="37" width="9.140625" style="7"/>
+    <col min="38" max="38" width="8.7109375"/>
+    <col min="39" max="1021" width="10.5703125" style="6"/>
+    <col min="1022" max="1025" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1022" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1024" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
@@ -2544,18 +2546,24 @@
       <c r="AI1" s="9">
         <v>29</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AJ1" s="9">
+        <v>30</v>
+      </c>
+      <c r="AK1" s="9">
         <v>31</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AMH1"/>
+      <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2572,7 +2580,7 @@
         <v>34</v>
       </c>
       <c r="F2" s="10">
-        <f>29-COUNTIF(G2:AI2,8)</f>
+        <f t="shared" ref="F2:F33" si="0">29-COUNTIF(G2:AI2,8)</f>
         <v>0</v>
       </c>
       <c r="G2" s="7">
@@ -2662,17 +2670,17 @@
       <c r="AI2" s="7">
         <v>8</v>
       </c>
-      <c r="AJ2" s="7">
+      <c r="AL2" s="7">
         <v>100</v>
       </c>
-      <c r="AK2" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="6">
+      <c r="AM2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2689,7 +2697,7 @@
         <v>34</v>
       </c>
       <c r="F3" s="10">
-        <f>29-COUNTIF(G3:AI3,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G3" s="7">
@@ -2779,17 +2787,17 @@
       <c r="AI3" s="7">
         <v>8</v>
       </c>
-      <c r="AJ3" s="7">
+      <c r="AL3" s="7">
         <v>100</v>
       </c>
-      <c r="AK3" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="6">
+      <c r="AM3" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2806,7 +2814,7 @@
         <v>34</v>
       </c>
       <c r="F4" s="10">
-        <f>29-COUNTIF(G4:AI4,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G4" s="7">
@@ -2896,17 +2904,17 @@
       <c r="AI4" s="7">
         <v>8</v>
       </c>
-      <c r="AJ4" s="7">
+      <c r="AL4" s="7">
         <v>100</v>
       </c>
-      <c r="AK4" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL4" s="6">
+      <c r="AM4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2923,7 +2931,7 @@
         <v>34</v>
       </c>
       <c r="F5" s="10">
-        <f>29-COUNTIF(G5:AI5,8)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G5" s="7" t="s">
@@ -3013,17 +3021,17 @@
       <c r="AI5" s="7">
         <v>8</v>
       </c>
-      <c r="AJ5" s="7">
+      <c r="AL5" s="7">
         <v>100</v>
       </c>
-      <c r="AK5" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL5" s="6">
+      <c r="AM5" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN5" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3040,7 +3048,7 @@
         <v>34</v>
       </c>
       <c r="F6" s="10">
-        <f>29-COUNTIF(G6:AI6,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G6" s="7">
@@ -3130,17 +3138,17 @@
       <c r="AI6" s="7">
         <v>8</v>
       </c>
-      <c r="AJ6" s="7">
+      <c r="AL6" s="7">
         <v>100</v>
       </c>
-      <c r="AK6" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL6" s="6">
+      <c r="AM6" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3157,7 +3165,7 @@
         <v>34</v>
       </c>
       <c r="F7" s="10">
-        <f>29-COUNTIF(G7:AI7,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G7" s="7">
@@ -3247,17 +3255,17 @@
       <c r="AI7" s="7">
         <v>8</v>
       </c>
-      <c r="AJ7" s="7">
+      <c r="AL7" s="7">
         <v>100</v>
       </c>
-      <c r="AK7" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL7" s="6">
+      <c r="AM7" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN7" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3274,7 +3282,7 @@
         <v>34</v>
       </c>
       <c r="F8" s="10">
-        <f>29-COUNTIF(G8:AI8,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G8" s="7">
@@ -3364,17 +3372,17 @@
       <c r="AI8" s="7">
         <v>8</v>
       </c>
-      <c r="AJ8" s="7">
+      <c r="AL8" s="7">
         <v>100</v>
       </c>
-      <c r="AK8" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL8" s="6">
+      <c r="AM8" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN8" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3391,7 +3399,7 @@
         <v>34</v>
       </c>
       <c r="F9" s="10">
-        <f>29-COUNTIF(G9:AI9,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G9" s="7">
@@ -3481,17 +3489,17 @@
       <c r="AI9" s="7">
         <v>8</v>
       </c>
-      <c r="AJ9" s="7">
+      <c r="AL9" s="7">
         <v>100</v>
       </c>
-      <c r="AK9" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL9" s="6">
+      <c r="AM9" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN9" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3508,7 +3516,7 @@
         <v>34</v>
       </c>
       <c r="F10" s="10">
-        <f>29-COUNTIF(G10:AI10,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G10" s="7">
@@ -3598,17 +3606,17 @@
       <c r="AI10" s="7">
         <v>8</v>
       </c>
-      <c r="AJ10" s="7">
+      <c r="AL10" s="7">
         <v>100</v>
       </c>
-      <c r="AK10" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL10" s="6">
+      <c r="AM10" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN10" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3625,7 +3633,7 @@
         <v>34</v>
       </c>
       <c r="F11" s="10">
-        <f>29-COUNTIF(G11:AI11,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G11" s="7">
@@ -3715,17 +3723,17 @@
       <c r="AI11" s="7">
         <v>8</v>
       </c>
-      <c r="AJ11" s="7">
+      <c r="AL11" s="7">
         <v>100</v>
       </c>
-      <c r="AK11" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL11" s="6">
+      <c r="AM11" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN11" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3742,7 +3750,7 @@
         <v>34</v>
       </c>
       <c r="F12" s="10">
-        <f>29-COUNTIF(G12:AI12,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G12" s="7">
@@ -3832,17 +3840,17 @@
       <c r="AI12" s="7">
         <v>8</v>
       </c>
-      <c r="AJ12" s="7">
+      <c r="AL12" s="7">
         <v>100</v>
       </c>
-      <c r="AK12" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL12" s="6">
+      <c r="AM12" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN12" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3859,7 +3867,7 @@
         <v>34</v>
       </c>
       <c r="F13" s="10">
-        <f>29-COUNTIF(G13:AI13,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G13" s="7">
@@ -3949,17 +3957,17 @@
       <c r="AI13" s="7">
         <v>8</v>
       </c>
-      <c r="AJ13" s="7">
+      <c r="AL13" s="7">
         <v>100</v>
       </c>
-      <c r="AK13" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL13" s="6">
+      <c r="AM13" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN13" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3976,7 +3984,7 @@
         <v>34</v>
       </c>
       <c r="F14" s="10">
-        <f>29-COUNTIF(G14:AI14,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G14" s="7">
@@ -4066,17 +4074,17 @@
       <c r="AI14" s="7">
         <v>8</v>
       </c>
-      <c r="AJ14" s="7">
+      <c r="AL14" s="7">
         <v>100</v>
       </c>
-      <c r="AK14" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL14" s="6">
+      <c r="AM14" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN14" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4093,7 +4101,7 @@
         <v>34</v>
       </c>
       <c r="F15" s="10">
-        <f>29-COUNTIF(G15:AI15,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G15" s="7">
@@ -4183,17 +4191,17 @@
       <c r="AI15" s="7">
         <v>8</v>
       </c>
-      <c r="AJ15" s="7">
+      <c r="AL15" s="7">
         <v>100</v>
       </c>
-      <c r="AK15" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL15" s="6">
+      <c r="AM15" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN15" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:1022" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4210,7 +4218,7 @@
         <v>34</v>
       </c>
       <c r="F16" s="10">
-        <f>29-COUNTIF(G16:AI16,8)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="G16" s="7">
@@ -4300,17 +4308,17 @@
       <c r="AI16" s="7">
         <v>8</v>
       </c>
-      <c r="AJ16" s="7">
+      <c r="AL16" s="7">
         <v>100</v>
       </c>
-      <c r="AK16" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL16" s="6">
+      <c r="AM16" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN16" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4327,7 +4335,7 @@
         <v>34</v>
       </c>
       <c r="F17" s="10">
-        <f>29-COUNTIF(G17:AI17,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G17" s="7">
@@ -4417,17 +4425,17 @@
       <c r="AI17" s="7">
         <v>8</v>
       </c>
-      <c r="AJ17" s="7">
+      <c r="AL17" s="7">
         <v>100</v>
       </c>
-      <c r="AK17" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL17" s="6">
+      <c r="AM17" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN17" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4444,7 +4452,7 @@
         <v>34</v>
       </c>
       <c r="F18" s="10">
-        <f>29-COUNTIF(G18:AI18,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G18" s="7">
@@ -4534,17 +4542,17 @@
       <c r="AI18" s="7">
         <v>8</v>
       </c>
-      <c r="AJ18" s="7">
+      <c r="AL18" s="7">
         <v>100</v>
       </c>
-      <c r="AK18" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL18" s="6">
+      <c r="AM18" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN18" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4561,7 +4569,7 @@
         <v>34</v>
       </c>
       <c r="F19" s="10">
-        <f>29-COUNTIF(G19:AI19,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G19" s="7">
@@ -4651,17 +4659,17 @@
       <c r="AI19" s="7">
         <v>8</v>
       </c>
-      <c r="AJ19" s="7">
+      <c r="AL19" s="7">
         <v>100</v>
       </c>
-      <c r="AK19" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL19" s="6">
+      <c r="AM19" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN19" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4678,7 +4686,7 @@
         <v>34</v>
       </c>
       <c r="F20" s="10">
-        <f>29-COUNTIF(G20:AI20,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G20" s="7">
@@ -4768,17 +4776,17 @@
       <c r="AI20" s="7">
         <v>8</v>
       </c>
-      <c r="AJ20" s="7">
+      <c r="AL20" s="7">
         <v>100</v>
       </c>
-      <c r="AK20" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL20" s="6">
+      <c r="AM20" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN20" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4795,7 +4803,7 @@
         <v>34</v>
       </c>
       <c r="F21" s="10">
-        <f>29-COUNTIF(G21:AI21,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G21" s="7">
@@ -4885,17 +4893,17 @@
       <c r="AI21" s="7">
         <v>8</v>
       </c>
-      <c r="AJ21" s="7">
+      <c r="AL21" s="7">
         <v>100</v>
       </c>
-      <c r="AK21" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL21" s="6">
+      <c r="AM21" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN21" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4912,7 +4920,7 @@
         <v>34</v>
       </c>
       <c r="F22" s="10">
-        <f>29-COUNTIF(G22:AI22,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G22" s="7">
@@ -5002,17 +5010,17 @@
       <c r="AI22" s="7">
         <v>8</v>
       </c>
-      <c r="AJ22" s="7">
+      <c r="AL22" s="7">
         <v>100</v>
       </c>
-      <c r="AK22" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL22" s="6">
+      <c r="AM22" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN22" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5029,7 +5037,7 @@
         <v>34</v>
       </c>
       <c r="F23" s="10">
-        <f>29-COUNTIF(G23:AI23,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G23" s="7">
@@ -5119,17 +5127,17 @@
       <c r="AI23" s="7">
         <v>8</v>
       </c>
-      <c r="AJ23" s="7">
+      <c r="AL23" s="7">
         <v>100</v>
       </c>
-      <c r="AK23" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL23" s="6">
+      <c r="AM23" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN23" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5146,7 +5154,7 @@
         <v>34</v>
       </c>
       <c r="F24" s="10">
-        <f>29-COUNTIF(G24:AI24,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G24" s="7">
@@ -5236,17 +5244,17 @@
       <c r="AI24" s="7">
         <v>8</v>
       </c>
-      <c r="AJ24" s="7">
+      <c r="AL24" s="7">
         <v>100</v>
       </c>
-      <c r="AK24" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL24" s="6">
+      <c r="AM24" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN24" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5263,7 +5271,7 @@
         <v>34</v>
       </c>
       <c r="F25" s="10">
-        <f>29-COUNTIF(G25:AI25,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G25" s="7">
@@ -5353,17 +5361,17 @@
       <c r="AI25" s="7">
         <v>8</v>
       </c>
-      <c r="AJ25" s="7">
+      <c r="AL25" s="7">
         <v>100</v>
       </c>
-      <c r="AK25" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL25" s="6">
+      <c r="AM25" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN25" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5380,7 +5388,7 @@
         <v>34</v>
       </c>
       <c r="F26" s="10">
-        <f>29-COUNTIF(G26:AI26,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G26" s="7">
@@ -5470,17 +5478,17 @@
       <c r="AI26" s="7">
         <v>8</v>
       </c>
-      <c r="AJ26" s="7">
+      <c r="AL26" s="7">
         <v>100</v>
       </c>
-      <c r="AK26" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL26" s="6">
+      <c r="AM26" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN26" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5497,7 +5505,7 @@
         <v>34</v>
       </c>
       <c r="F27" s="10">
-        <f>29-COUNTIF(G27:AI27,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G27" s="7">
@@ -5587,17 +5595,17 @@
       <c r="AI27" s="7">
         <v>8</v>
       </c>
-      <c r="AJ27" s="7">
+      <c r="AL27" s="7">
         <v>100</v>
       </c>
-      <c r="AK27" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL27" s="6">
+      <c r="AM27" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN27" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5614,7 +5622,7 @@
         <v>34</v>
       </c>
       <c r="F28" s="10">
-        <f>29-COUNTIF(G28:AI28,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G28" s="7">
@@ -5704,17 +5712,17 @@
       <c r="AI28" s="7">
         <v>8</v>
       </c>
-      <c r="AJ28" s="7">
+      <c r="AL28" s="7">
         <v>100</v>
       </c>
-      <c r="AK28" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL28" s="6">
+      <c r="AM28" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN28" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5731,7 +5739,7 @@
         <v>34</v>
       </c>
       <c r="F29" s="10">
-        <f>29-COUNTIF(G29:AI29,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G29" s="7">
@@ -5821,17 +5829,17 @@
       <c r="AI29" s="7">
         <v>8</v>
       </c>
-      <c r="AJ29" s="7">
+      <c r="AL29" s="7">
         <v>100</v>
       </c>
-      <c r="AK29" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL29" s="6">
+      <c r="AM29" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN29" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5848,7 +5856,7 @@
         <v>34</v>
       </c>
       <c r="F30" s="10">
-        <f>29-COUNTIF(G30:AI30,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G30" s="7">
@@ -5938,17 +5946,17 @@
       <c r="AI30" s="7">
         <v>8</v>
       </c>
-      <c r="AJ30" s="7">
+      <c r="AL30" s="7">
         <v>100</v>
       </c>
-      <c r="AK30" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL30" s="6">
+      <c r="AM30" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN30" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5965,7 +5973,7 @@
         <v>34</v>
       </c>
       <c r="F31" s="10">
-        <f>29-COUNTIF(G31:AI31,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G31" s="7">
@@ -6055,17 +6063,17 @@
       <c r="AI31" s="7">
         <v>8</v>
       </c>
-      <c r="AJ31" s="7">
+      <c r="AL31" s="7">
         <v>100</v>
       </c>
-      <c r="AK31" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL31" s="6">
+      <c r="AM31" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN31" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -6082,7 +6090,7 @@
         <v>34</v>
       </c>
       <c r="F32" s="10">
-        <f>29-COUNTIF(G32:AI32,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G32" s="7">
@@ -6172,17 +6180,17 @@
       <c r="AI32" s="7">
         <v>8</v>
       </c>
-      <c r="AJ32" s="7">
+      <c r="AL32" s="7">
         <v>100</v>
       </c>
-      <c r="AK32" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL32" s="6">
+      <c r="AM32" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN32" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -6199,7 +6207,7 @@
         <v>34</v>
       </c>
       <c r="F33" s="10">
-        <f>29-COUNTIF(G33:AI33,8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G33" s="7">
@@ -6289,17 +6297,17 @@
       <c r="AI33" s="7">
         <v>8</v>
       </c>
-      <c r="AJ33" s="7">
+      <c r="AL33" s="7">
         <v>100</v>
       </c>
-      <c r="AK33" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL33" s="6">
+      <c r="AM33" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN33" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -6316,7 +6324,7 @@
         <v>34</v>
       </c>
       <c r="F34" s="10">
-        <f>29-COUNTIF(G34:AI34,8)</f>
+        <f t="shared" ref="F34:F65" si="1">29-COUNTIF(G34:AI34,8)</f>
         <v>0</v>
       </c>
       <c r="G34" s="7">
@@ -6406,17 +6414,17 @@
       <c r="AI34" s="7">
         <v>8</v>
       </c>
-      <c r="AJ34" s="7">
+      <c r="AL34" s="7">
         <v>100</v>
       </c>
-      <c r="AK34" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL34" s="6">
+      <c r="AM34" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN34" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -6433,7 +6441,7 @@
         <v>34</v>
       </c>
       <c r="F35" s="10">
-        <f>29-COUNTIF(G35:AI35,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G35" s="7">
@@ -6523,17 +6531,17 @@
       <c r="AI35" s="7">
         <v>8</v>
       </c>
-      <c r="AJ35" s="7">
+      <c r="AL35" s="7">
         <v>100</v>
       </c>
-      <c r="AK35" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL35" s="6">
+      <c r="AM35" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN35" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -6550,7 +6558,7 @@
         <v>34</v>
       </c>
       <c r="F36" s="10">
-        <f>29-COUNTIF(G36:AI36,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G36" s="7">
@@ -6640,17 +6648,17 @@
       <c r="AI36" s="7">
         <v>8</v>
       </c>
-      <c r="AJ36" s="7">
+      <c r="AL36" s="7">
         <v>100</v>
       </c>
-      <c r="AK36" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL36" s="6">
+      <c r="AM36" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN36" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -6667,7 +6675,7 @@
         <v>34</v>
       </c>
       <c r="F37" s="10">
-        <f>29-COUNTIF(G37:AI37,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G37" s="7">
@@ -6757,17 +6765,17 @@
       <c r="AI37" s="7">
         <v>8</v>
       </c>
-      <c r="AJ37" s="7">
+      <c r="AL37" s="7">
         <v>100</v>
       </c>
-      <c r="AK37" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL37" s="6">
+      <c r="AM37" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN37" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -6784,7 +6792,7 @@
         <v>34</v>
       </c>
       <c r="F38" s="10">
-        <f>29-COUNTIF(G38:AI38,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G38" s="7">
@@ -6874,17 +6882,17 @@
       <c r="AI38" s="7">
         <v>8</v>
       </c>
-      <c r="AJ38" s="7">
+      <c r="AL38" s="7">
         <v>100</v>
       </c>
-      <c r="AK38" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL38" s="6">
+      <c r="AM38" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN38" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -6901,7 +6909,7 @@
         <v>34</v>
       </c>
       <c r="F39" s="10">
-        <f>29-COUNTIF(G39:AI39,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G39" s="7">
@@ -6991,17 +6999,17 @@
       <c r="AI39" s="7">
         <v>8</v>
       </c>
-      <c r="AJ39" s="7">
+      <c r="AL39" s="7">
         <v>100</v>
       </c>
-      <c r="AK39" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL39" s="6">
+      <c r="AM39" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN39" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -7018,7 +7026,7 @@
         <v>34</v>
       </c>
       <c r="F40" s="10">
-        <f>29-COUNTIF(G40:AI40,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G40" s="7">
@@ -7108,17 +7116,17 @@
       <c r="AI40" s="7">
         <v>8</v>
       </c>
-      <c r="AJ40" s="7">
+      <c r="AL40" s="7">
         <v>100</v>
       </c>
-      <c r="AK40" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL40" s="6">
+      <c r="AM40" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN40" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -7135,7 +7143,7 @@
         <v>34</v>
       </c>
       <c r="F41" s="10">
-        <f>29-COUNTIF(G41:AI41,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G41" s="7">
@@ -7225,17 +7233,17 @@
       <c r="AI41" s="7">
         <v>8</v>
       </c>
-      <c r="AJ41" s="7">
+      <c r="AL41" s="7">
         <v>100</v>
       </c>
-      <c r="AK41" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL41" s="6">
+      <c r="AM41" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN41" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -7252,7 +7260,7 @@
         <v>34</v>
       </c>
       <c r="F42" s="10">
-        <f>29-COUNTIF(G42:AI42,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G42" s="7">
@@ -7342,17 +7350,17 @@
       <c r="AI42" s="7">
         <v>8</v>
       </c>
-      <c r="AJ42" s="7">
+      <c r="AL42" s="7">
         <v>100</v>
       </c>
-      <c r="AK42" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL42" s="6">
+      <c r="AM42" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN42" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -7369,7 +7377,7 @@
         <v>34</v>
       </c>
       <c r="F43" s="10">
-        <f>29-COUNTIF(G43:AI43,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G43" s="7">
@@ -7459,17 +7467,17 @@
       <c r="AI43" s="7">
         <v>8</v>
       </c>
-      <c r="AJ43" s="7">
+      <c r="AL43" s="7">
         <v>100</v>
       </c>
-      <c r="AK43" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL43" s="6">
+      <c r="AM43" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN43" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -7486,7 +7494,7 @@
         <v>34</v>
       </c>
       <c r="F44" s="10">
-        <f>29-COUNTIF(G44:AI44,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G44" s="7">
@@ -7576,17 +7584,17 @@
       <c r="AI44" s="7">
         <v>8</v>
       </c>
-      <c r="AJ44" s="7">
+      <c r="AL44" s="7">
         <v>100</v>
       </c>
-      <c r="AK44" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL44" s="6">
+      <c r="AM44" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN44" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -7603,7 +7611,7 @@
         <v>34</v>
       </c>
       <c r="F45" s="10">
-        <f>29-COUNTIF(G45:AI45,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G45" s="7">
@@ -7693,17 +7701,17 @@
       <c r="AI45" s="7">
         <v>8</v>
       </c>
-      <c r="AJ45" s="7">
+      <c r="AL45" s="7">
         <v>100</v>
       </c>
-      <c r="AK45" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL45" s="6">
+      <c r="AM45" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN45" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -7720,7 +7728,7 @@
         <v>34</v>
       </c>
       <c r="F46" s="10">
-        <f>29-COUNTIF(G46:AI46,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G46" s="7">
@@ -7810,17 +7818,17 @@
       <c r="AI46" s="7">
         <v>8</v>
       </c>
-      <c r="AJ46" s="7">
+      <c r="AL46" s="7">
         <v>100</v>
       </c>
-      <c r="AK46" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL46" s="6">
+      <c r="AM46" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN46" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -7837,7 +7845,7 @@
         <v>34</v>
       </c>
       <c r="F47" s="10">
-        <f>29-COUNTIF(G47:AI47,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G47" s="7">
@@ -7927,17 +7935,17 @@
       <c r="AI47" s="7">
         <v>8</v>
       </c>
-      <c r="AJ47" s="7">
+      <c r="AL47" s="7">
         <v>100</v>
       </c>
-      <c r="AK47" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL47" s="6">
+      <c r="AM47" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN47" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -7954,7 +7962,7 @@
         <v>34</v>
       </c>
       <c r="F48" s="10">
-        <f>29-COUNTIF(G48:AI48,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G48" s="7">
@@ -8044,17 +8052,17 @@
       <c r="AI48" s="7">
         <v>8</v>
       </c>
-      <c r="AJ48" s="7">
+      <c r="AL48" s="7">
         <v>100</v>
       </c>
-      <c r="AK48" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL48" s="6">
+      <c r="AM48" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN48" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -8071,7 +8079,7 @@
         <v>34</v>
       </c>
       <c r="F49" s="10">
-        <f>29-COUNTIF(G49:AI49,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G49" s="7">
@@ -8161,17 +8169,17 @@
       <c r="AI49" s="7">
         <v>8</v>
       </c>
-      <c r="AJ49" s="7">
+      <c r="AL49" s="7">
         <v>100</v>
       </c>
-      <c r="AK49" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL49" s="6">
+      <c r="AM49" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN49" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -8188,7 +8196,7 @@
         <v>34</v>
       </c>
       <c r="F50" s="10">
-        <f>29-COUNTIF(G50:AI50,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G50" s="7">
@@ -8278,17 +8286,17 @@
       <c r="AI50" s="7">
         <v>8</v>
       </c>
-      <c r="AJ50" s="7">
+      <c r="AL50" s="7">
         <v>100</v>
       </c>
-      <c r="AK50" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL50" s="6">
+      <c r="AM50" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN50" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -8305,7 +8313,7 @@
         <v>34</v>
       </c>
       <c r="F51" s="10">
-        <f>29-COUNTIF(G51:AI51,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G51" s="7">
@@ -8395,17 +8403,17 @@
       <c r="AI51" s="7">
         <v>8</v>
       </c>
-      <c r="AJ51" s="7">
+      <c r="AL51" s="7">
         <v>100</v>
       </c>
-      <c r="AK51" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL51" s="6">
+      <c r="AM51" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN51" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -8422,7 +8430,7 @@
         <v>34</v>
       </c>
       <c r="F52" s="10">
-        <f>29-COUNTIF(G52:AI52,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G52" s="7">
@@ -8512,17 +8520,17 @@
       <c r="AI52" s="7">
         <v>8</v>
       </c>
-      <c r="AJ52" s="7">
+      <c r="AL52" s="7">
         <v>100</v>
       </c>
-      <c r="AK52" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL52" s="6">
+      <c r="AM52" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN52" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -8539,7 +8547,7 @@
         <v>34</v>
       </c>
       <c r="F53" s="10">
-        <f>29-COUNTIF(G53:AI53,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G53" s="7">
@@ -8629,17 +8637,17 @@
       <c r="AI53" s="7">
         <v>8</v>
       </c>
-      <c r="AJ53" s="7">
+      <c r="AL53" s="7">
         <v>100</v>
       </c>
-      <c r="AK53" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL53" s="6">
+      <c r="AM53" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN53" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -8656,7 +8664,7 @@
         <v>34</v>
       </c>
       <c r="F54" s="10">
-        <f>29-COUNTIF(G54:AI54,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G54" s="7">
@@ -8746,17 +8754,17 @@
       <c r="AI54" s="7">
         <v>8</v>
       </c>
-      <c r="AJ54" s="7">
+      <c r="AL54" s="7">
         <v>100</v>
       </c>
-      <c r="AK54" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL54" s="6">
+      <c r="AM54" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN54" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -8773,7 +8781,7 @@
         <v>34</v>
       </c>
       <c r="F55" s="10">
-        <f>29-COUNTIF(G55:AI55,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G55" s="7">
@@ -8863,17 +8871,17 @@
       <c r="AI55" s="7">
         <v>8</v>
       </c>
-      <c r="AJ55" s="7">
+      <c r="AL55" s="7">
         <v>100</v>
       </c>
-      <c r="AK55" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL55" s="6">
+      <c r="AM55" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN55" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -8890,7 +8898,7 @@
         <v>34</v>
       </c>
       <c r="F56" s="10">
-        <f>29-COUNTIF(G56:AI56,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G56" s="7">
@@ -8980,17 +8988,17 @@
       <c r="AI56" s="7">
         <v>8</v>
       </c>
-      <c r="AJ56" s="7">
+      <c r="AL56" s="7">
         <v>100</v>
       </c>
-      <c r="AK56" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL56" s="6">
+      <c r="AM56" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN56" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -9007,7 +9015,7 @@
         <v>34</v>
       </c>
       <c r="F57" s="10">
-        <f>29-COUNTIF(G57:AI57,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G57" s="7">
@@ -9097,17 +9105,17 @@
       <c r="AI57" s="7">
         <v>8</v>
       </c>
-      <c r="AJ57" s="7">
+      <c r="AL57" s="7">
         <v>100</v>
       </c>
-      <c r="AK57" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL57" s="6">
+      <c r="AM57" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN57" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -9124,7 +9132,7 @@
         <v>34</v>
       </c>
       <c r="F58" s="10">
-        <f>29-COUNTIF(G58:AI58,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G58" s="7">
@@ -9214,17 +9222,17 @@
       <c r="AI58" s="7">
         <v>8</v>
       </c>
-      <c r="AJ58" s="7">
+      <c r="AL58" s="7">
         <v>100</v>
       </c>
-      <c r="AK58" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL58" s="6">
+      <c r="AM58" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN58" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -9241,7 +9249,7 @@
         <v>34</v>
       </c>
       <c r="F59" s="10">
-        <f>29-COUNTIF(G59:AI59,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G59" s="7">
@@ -9331,17 +9339,17 @@
       <c r="AI59" s="7">
         <v>8</v>
       </c>
-      <c r="AJ59" s="7">
+      <c r="AL59" s="7">
         <v>100</v>
       </c>
-      <c r="AK59" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL59" s="6">
+      <c r="AM59" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN59" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -9358,7 +9366,7 @@
         <v>34</v>
       </c>
       <c r="F60" s="10">
-        <f>29-COUNTIF(G60:AI60,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G60" s="7">
@@ -9448,17 +9456,17 @@
       <c r="AI60" s="7">
         <v>8</v>
       </c>
-      <c r="AJ60" s="7">
+      <c r="AL60" s="7">
         <v>100</v>
       </c>
-      <c r="AK60" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL60" s="6">
+      <c r="AM60" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN60" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -9475,7 +9483,7 @@
         <v>34</v>
       </c>
       <c r="F61" s="10">
-        <f>29-COUNTIF(G61:AI61,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G61" s="7">
@@ -9565,17 +9573,17 @@
       <c r="AI61" s="7">
         <v>8</v>
       </c>
-      <c r="AJ61" s="7">
+      <c r="AL61" s="7">
         <v>100</v>
       </c>
-      <c r="AK61" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL61" s="6">
+      <c r="AM61" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN61" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -9592,7 +9600,7 @@
         <v>34</v>
       </c>
       <c r="F62" s="10">
-        <f>29-COUNTIF(G62:AI62,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G62" s="7">
@@ -9682,17 +9690,17 @@
       <c r="AI62" s="7">
         <v>8</v>
       </c>
-      <c r="AJ62" s="7">
+      <c r="AL62" s="7">
         <v>100</v>
       </c>
-      <c r="AK62" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL62" s="6">
+      <c r="AM62" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN62" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -9709,7 +9717,7 @@
         <v>34</v>
       </c>
       <c r="F63" s="10">
-        <f>29-COUNTIF(G63:AI63,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G63" s="7">
@@ -9799,17 +9807,17 @@
       <c r="AI63" s="7">
         <v>8</v>
       </c>
-      <c r="AJ63" s="7">
+      <c r="AL63" s="7">
         <v>100</v>
       </c>
-      <c r="AK63" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL63" s="6">
+      <c r="AM63" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN63" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -9826,7 +9834,7 @@
         <v>34</v>
       </c>
       <c r="F64" s="10">
-        <f>29-COUNTIF(G64:AI64,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G64" s="7">
@@ -9916,17 +9924,17 @@
       <c r="AI64" s="7">
         <v>8</v>
       </c>
-      <c r="AJ64" s="7">
+      <c r="AL64" s="7">
         <v>100</v>
       </c>
-      <c r="AK64" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL64" s="6">
+      <c r="AM64" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN64" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -9943,7 +9951,7 @@
         <v>34</v>
       </c>
       <c r="F65" s="10">
-        <f>29-COUNTIF(G65:AI65,8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G65" s="7">
@@ -10033,17 +10041,17 @@
       <c r="AI65" s="7">
         <v>8</v>
       </c>
-      <c r="AJ65" s="7">
+      <c r="AL65" s="7">
         <v>100</v>
       </c>
-      <c r="AK65" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL65" s="6">
+      <c r="AM65" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN65" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -10060,7 +10068,7 @@
         <v>34</v>
       </c>
       <c r="F66" s="10">
-        <f>29-COUNTIF(G66:AI66,8)</f>
+        <f t="shared" ref="F66:F97" si="2">29-COUNTIF(G66:AI66,8)</f>
         <v>0</v>
       </c>
       <c r="G66" s="7">
@@ -10150,17 +10158,17 @@
       <c r="AI66" s="7">
         <v>8</v>
       </c>
-      <c r="AJ66" s="7">
+      <c r="AL66" s="7">
         <v>100</v>
       </c>
-      <c r="AK66" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL66" s="6">
+      <c r="AM66" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN66" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -10177,7 +10185,7 @@
         <v>34</v>
       </c>
       <c r="F67" s="10">
-        <f>29-COUNTIF(G67:AI67,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G67" s="7">
@@ -10267,17 +10275,17 @@
       <c r="AI67" s="7">
         <v>8</v>
       </c>
-      <c r="AJ67" s="7">
+      <c r="AL67" s="7">
         <v>100</v>
       </c>
-      <c r="AK67" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL67" s="6">
+      <c r="AM67" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN67" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -10294,7 +10302,7 @@
         <v>34</v>
       </c>
       <c r="F68" s="10">
-        <f>29-COUNTIF(G68:AI68,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G68" s="7">
@@ -10384,17 +10392,17 @@
       <c r="AI68" s="7">
         <v>8</v>
       </c>
-      <c r="AJ68" s="7">
+      <c r="AL68" s="7">
         <v>100</v>
       </c>
-      <c r="AK68" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL68" s="6">
+      <c r="AM68" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN68" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -10411,7 +10419,7 @@
         <v>34</v>
       </c>
       <c r="F69" s="10">
-        <f>29-COUNTIF(G69:AI69,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G69" s="7">
@@ -10501,17 +10509,17 @@
       <c r="AI69" s="7">
         <v>8</v>
       </c>
-      <c r="AJ69" s="7">
+      <c r="AL69" s="7">
         <v>100</v>
       </c>
-      <c r="AK69" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL69" s="6">
+      <c r="AM69" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN69" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -10528,7 +10536,7 @@
         <v>34</v>
       </c>
       <c r="F70" s="10">
-        <f>29-COUNTIF(G70:AI70,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G70" s="7">
@@ -10618,17 +10626,17 @@
       <c r="AI70" s="7">
         <v>8</v>
       </c>
-      <c r="AJ70" s="7">
+      <c r="AL70" s="7">
         <v>100</v>
       </c>
-      <c r="AK70" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL70" s="6">
+      <c r="AM70" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN70" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -10645,7 +10653,7 @@
         <v>34</v>
       </c>
       <c r="F71" s="10">
-        <f>29-COUNTIF(G71:AI71,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G71" s="7">
@@ -10735,17 +10743,17 @@
       <c r="AI71" s="7">
         <v>8</v>
       </c>
-      <c r="AJ71" s="7">
+      <c r="AL71" s="7">
         <v>100</v>
       </c>
-      <c r="AK71" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL71" s="6">
+      <c r="AM71" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN71" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -10762,7 +10770,7 @@
         <v>34</v>
       </c>
       <c r="F72" s="10">
-        <f>29-COUNTIF(G72:AI72,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G72" s="7">
@@ -10852,17 +10860,17 @@
       <c r="AI72" s="7">
         <v>8</v>
       </c>
-      <c r="AJ72" s="7">
+      <c r="AL72" s="7">
         <v>100</v>
       </c>
-      <c r="AK72" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL72" s="6">
+      <c r="AM72" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN72" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -10879,7 +10887,7 @@
         <v>34</v>
       </c>
       <c r="F73" s="10">
-        <f>29-COUNTIF(G73:AI73,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G73" s="7">
@@ -10969,17 +10977,17 @@
       <c r="AI73" s="7">
         <v>8</v>
       </c>
-      <c r="AJ73" s="7">
+      <c r="AL73" s="7">
         <v>100</v>
       </c>
-      <c r="AK73" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL73" s="6">
+      <c r="AM73" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN73" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -10996,7 +11004,7 @@
         <v>34</v>
       </c>
       <c r="F74" s="10">
-        <f>29-COUNTIF(G74:AI74,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G74" s="7">
@@ -11086,17 +11094,17 @@
       <c r="AI74" s="7">
         <v>8</v>
       </c>
-      <c r="AJ74" s="7">
+      <c r="AL74" s="7">
         <v>100</v>
       </c>
-      <c r="AK74" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL74" s="6">
+      <c r="AM74" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN74" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -11113,7 +11121,7 @@
         <v>34</v>
       </c>
       <c r="F75" s="10">
-        <f>29-COUNTIF(G75:AI75,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G75" s="7">
@@ -11203,17 +11211,17 @@
       <c r="AI75" s="7">
         <v>8</v>
       </c>
-      <c r="AJ75" s="7">
+      <c r="AL75" s="7">
         <v>100</v>
       </c>
-      <c r="AK75" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL75" s="6">
+      <c r="AM75" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN75" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -11230,7 +11238,7 @@
         <v>34</v>
       </c>
       <c r="F76" s="10">
-        <f>29-COUNTIF(G76:AI76,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G76" s="7">
@@ -11320,17 +11328,17 @@
       <c r="AI76" s="7">
         <v>8</v>
       </c>
-      <c r="AJ76" s="7">
+      <c r="AL76" s="7">
         <v>100</v>
       </c>
-      <c r="AK76" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL76" s="6">
+      <c r="AM76" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN76" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -11347,7 +11355,7 @@
         <v>34</v>
       </c>
       <c r="F77" s="10">
-        <f>29-COUNTIF(G77:AI77,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G77" s="7">
@@ -11437,17 +11445,17 @@
       <c r="AI77" s="7">
         <v>8</v>
       </c>
-      <c r="AJ77" s="7">
+      <c r="AL77" s="7">
         <v>100</v>
       </c>
-      <c r="AK77" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL77" s="6">
+      <c r="AM77" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN77" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -11464,7 +11472,7 @@
         <v>34</v>
       </c>
       <c r="F78" s="10">
-        <f>29-COUNTIF(G78:AI78,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G78" s="7">
@@ -11554,17 +11562,17 @@
       <c r="AI78" s="7">
         <v>8</v>
       </c>
-      <c r="AJ78" s="7">
+      <c r="AL78" s="7">
         <v>100</v>
       </c>
-      <c r="AK78" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL78" s="6">
+      <c r="AM78" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN78" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -11581,7 +11589,7 @@
         <v>34</v>
       </c>
       <c r="F79" s="10">
-        <f>29-COUNTIF(G79:AI79,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G79" s="7">
@@ -11671,17 +11679,17 @@
       <c r="AI79" s="7">
         <v>8</v>
       </c>
-      <c r="AJ79" s="7">
+      <c r="AL79" s="7">
         <v>100</v>
       </c>
-      <c r="AK79" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL79" s="6">
+      <c r="AM79" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN79" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -11698,7 +11706,7 @@
         <v>34</v>
       </c>
       <c r="F80" s="10">
-        <f>29-COUNTIF(G80:AI80,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G80" s="7">
@@ -11788,17 +11796,17 @@
       <c r="AI80" s="7">
         <v>8</v>
       </c>
-      <c r="AJ80" s="7">
+      <c r="AL80" s="7">
         <v>100</v>
       </c>
-      <c r="AK80" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL80" s="6">
+      <c r="AM80" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN80" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -11815,7 +11823,7 @@
         <v>34</v>
       </c>
       <c r="F81" s="10">
-        <f>29-COUNTIF(G81:AI81,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G81" s="7">
@@ -11905,17 +11913,17 @@
       <c r="AI81" s="7">
         <v>8</v>
       </c>
-      <c r="AJ81" s="7">
+      <c r="AL81" s="7">
         <v>100</v>
       </c>
-      <c r="AK81" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL81" s="6">
+      <c r="AM81" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN81" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -11932,7 +11940,7 @@
         <v>34</v>
       </c>
       <c r="F82" s="10">
-        <f>29-COUNTIF(G82:AI82,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G82" s="7">
@@ -12022,17 +12030,17 @@
       <c r="AI82" s="7">
         <v>8</v>
       </c>
-      <c r="AJ82" s="7">
+      <c r="AL82" s="7">
         <v>100</v>
       </c>
-      <c r="AK82" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL82" s="6">
+      <c r="AM82" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN82" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -12049,7 +12057,7 @@
         <v>34</v>
       </c>
       <c r="F83" s="10">
-        <f>29-COUNTIF(G83:AI83,8)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G83" s="7" t="s">
@@ -12139,17 +12147,17 @@
       <c r="AI83" s="7">
         <v>8</v>
       </c>
-      <c r="AJ83" s="7">
+      <c r="AL83" s="7">
         <v>100</v>
       </c>
-      <c r="AK83" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL83" s="6">
+      <c r="AM83" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN83" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -12166,7 +12174,7 @@
         <v>34</v>
       </c>
       <c r="F84" s="10">
-        <f>29-COUNTIF(G84:AI84,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G84" s="7">
@@ -12256,17 +12264,17 @@
       <c r="AI84" s="7">
         <v>8</v>
       </c>
-      <c r="AJ84" s="7">
+      <c r="AL84" s="7">
         <v>100</v>
       </c>
-      <c r="AK84" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL84" s="6">
+      <c r="AM84" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN84" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -12283,7 +12291,7 @@
         <v>34</v>
       </c>
       <c r="F85" s="10">
-        <f>29-COUNTIF(G85:AI85,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G85" s="7">
@@ -12373,17 +12381,17 @@
       <c r="AI85" s="7">
         <v>8</v>
       </c>
-      <c r="AJ85" s="7">
+      <c r="AL85" s="7">
         <v>100</v>
       </c>
-      <c r="AK85" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL85" s="6">
+      <c r="AM85" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN85" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -12400,7 +12408,7 @@
         <v>34</v>
       </c>
       <c r="F86" s="10">
-        <f>29-COUNTIF(G86:AI86,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G86" s="7">
@@ -12490,17 +12498,17 @@
       <c r="AI86" s="7">
         <v>8</v>
       </c>
-      <c r="AJ86" s="7">
+      <c r="AL86" s="7">
         <v>100</v>
       </c>
-      <c r="AK86" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL86" s="6">
+      <c r="AM86" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN86" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -12517,7 +12525,7 @@
         <v>34</v>
       </c>
       <c r="F87" s="10">
-        <f>29-COUNTIF(G87:AI87,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G87" s="7">
@@ -12607,17 +12615,17 @@
       <c r="AI87" s="7">
         <v>8</v>
       </c>
-      <c r="AJ87" s="7">
+      <c r="AL87" s="7">
         <v>100</v>
       </c>
-      <c r="AK87" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL87" s="6">
+      <c r="AM87" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN87" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -12634,7 +12642,7 @@
         <v>34</v>
       </c>
       <c r="F88" s="10">
-        <f>29-COUNTIF(G88:AI88,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G88" s="7">
@@ -12724,17 +12732,17 @@
       <c r="AI88" s="7">
         <v>8</v>
       </c>
-      <c r="AJ88" s="7">
+      <c r="AL88" s="7">
         <v>100</v>
       </c>
-      <c r="AK88" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL88" s="6">
+      <c r="AM88" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN88" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -12751,7 +12759,7 @@
         <v>34</v>
       </c>
       <c r="F89" s="10">
-        <f>29-COUNTIF(G89:AI89,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G89" s="7">
@@ -12841,17 +12849,17 @@
       <c r="AI89" s="7">
         <v>8</v>
       </c>
-      <c r="AJ89" s="7">
+      <c r="AL89" s="7">
         <v>100</v>
       </c>
-      <c r="AK89" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL89" s="6">
+      <c r="AM89" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN89" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -12868,7 +12876,7 @@
         <v>34</v>
       </c>
       <c r="F90" s="10">
-        <f>29-COUNTIF(G90:AI90,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G90" s="7">
@@ -12958,17 +12966,17 @@
       <c r="AI90" s="7">
         <v>8</v>
       </c>
-      <c r="AJ90" s="7">
+      <c r="AL90" s="7">
         <v>100</v>
       </c>
-      <c r="AK90" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL90" s="6">
+      <c r="AM90" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN90" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -12985,7 +12993,7 @@
         <v>34</v>
       </c>
       <c r="F91" s="10">
-        <f>29-COUNTIF(G91:AI91,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G91" s="7">
@@ -13075,17 +13083,17 @@
       <c r="AI91" s="7">
         <v>8</v>
       </c>
-      <c r="AJ91" s="7">
+      <c r="AL91" s="7">
         <v>100</v>
       </c>
-      <c r="AK91" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL91" s="6">
+      <c r="AM91" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN91" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -13102,7 +13110,7 @@
         <v>34</v>
       </c>
       <c r="F92" s="10">
-        <f>29-COUNTIF(G92:AI92,8)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="G92" s="7" t="s">
@@ -13192,17 +13200,17 @@
       <c r="AI92" s="7">
         <v>8</v>
       </c>
-      <c r="AJ92" s="7">
+      <c r="AL92" s="7">
         <v>100</v>
       </c>
-      <c r="AK92" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL92" s="6">
+      <c r="AM92" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN92" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -13219,7 +13227,7 @@
         <v>34</v>
       </c>
       <c r="F93" s="10">
-        <f>29-COUNTIF(G93:AI93,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G93" s="7">
@@ -13309,17 +13317,17 @@
       <c r="AI93" s="7">
         <v>8</v>
       </c>
-      <c r="AJ93" s="7">
+      <c r="AL93" s="7">
         <v>100</v>
       </c>
-      <c r="AK93" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL93" s="6">
+      <c r="AM93" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN93" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -13336,7 +13344,7 @@
         <v>34</v>
       </c>
       <c r="F94" s="10">
-        <f>29-COUNTIF(G94:AI94,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G94" s="7">
@@ -13426,17 +13434,17 @@
       <c r="AI94" s="7">
         <v>8</v>
       </c>
-      <c r="AJ94" s="7">
+      <c r="AL94" s="7">
         <v>100</v>
       </c>
-      <c r="AK94" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL94" s="6">
+      <c r="AM94" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN94" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -13453,7 +13461,7 @@
         <v>34</v>
       </c>
       <c r="F95" s="10">
-        <f>29-COUNTIF(G95:AI95,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G95" s="7">
@@ -13543,17 +13551,17 @@
       <c r="AI95" s="7">
         <v>8</v>
       </c>
-      <c r="AJ95" s="7">
+      <c r="AL95" s="7">
         <v>100</v>
       </c>
-      <c r="AK95" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL95" s="6">
+      <c r="AM95" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN95" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -13570,7 +13578,7 @@
         <v>34</v>
       </c>
       <c r="F96" s="10">
-        <f>29-COUNTIF(G96:AI96,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G96" s="7">
@@ -13660,17 +13668,17 @@
       <c r="AI96" s="7">
         <v>8</v>
       </c>
-      <c r="AJ96" s="7">
+      <c r="AL96" s="7">
         <v>100</v>
       </c>
-      <c r="AK96" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL96" s="6">
+      <c r="AM96" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN96" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -13687,7 +13695,7 @@
         <v>34</v>
       </c>
       <c r="F97" s="10">
-        <f>29-COUNTIF(G97:AI97,8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G97" s="7">
@@ -13777,17 +13785,17 @@
       <c r="AI97" s="7">
         <v>8</v>
       </c>
-      <c r="AJ97" s="7">
+      <c r="AL97" s="7">
         <v>100</v>
       </c>
-      <c r="AK97" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL97" s="6">
+      <c r="AM97" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN97" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -13804,7 +13812,7 @@
         <v>34</v>
       </c>
       <c r="F98" s="10">
-        <f>29-COUNTIF(G98:AI98,8)</f>
+        <f t="shared" ref="F98:F129" si="3">29-COUNTIF(G98:AI98,8)</f>
         <v>0</v>
       </c>
       <c r="G98" s="7">
@@ -13894,17 +13902,17 @@
       <c r="AI98" s="7">
         <v>8</v>
       </c>
-      <c r="AJ98" s="7">
+      <c r="AL98" s="7">
         <v>100</v>
       </c>
-      <c r="AK98" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL98" s="6">
+      <c r="AM98" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN98" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -13921,7 +13929,7 @@
         <v>34</v>
       </c>
       <c r="F99" s="10">
-        <f>29-COUNTIF(G99:AI99,8)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G99" s="7">
@@ -14011,17 +14019,17 @@
       <c r="AI99" s="7">
         <v>8</v>
       </c>
-      <c r="AJ99" s="7">
+      <c r="AL99" s="7">
         <v>100</v>
       </c>
-      <c r="AK99" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL99" s="6">
+      <c r="AM99" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN99" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -14038,7 +14046,7 @@
         <v>34</v>
       </c>
       <c r="F100" s="10">
-        <f>29-COUNTIF(G100:AI100,8)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G100" s="7">
@@ -14128,17 +14136,17 @@
       <c r="AI100" s="7">
         <v>8</v>
       </c>
-      <c r="AJ100" s="7">
+      <c r="AL100" s="7">
         <v>100</v>
       </c>
-      <c r="AK100" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL100" s="6">
+      <c r="AM100" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN100" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -14155,7 +14163,7 @@
         <v>34</v>
       </c>
       <c r="F101" s="10">
-        <f>29-COUNTIF(G101:AI101,8)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G101" s="7">
@@ -14245,17 +14253,17 @@
       <c r="AI101" s="7">
         <v>8</v>
       </c>
-      <c r="AJ101" s="7">
+      <c r="AL101" s="7">
         <v>100</v>
       </c>
-      <c r="AK101" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL101" s="6">
+      <c r="AM101" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN101" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -14272,7 +14280,7 @@
         <v>34</v>
       </c>
       <c r="F102" s="10">
-        <f>29-COUNTIF(G102:AI102,8)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G102" s="7">
@@ -14362,17 +14370,17 @@
       <c r="AI102" s="7">
         <v>8</v>
       </c>
-      <c r="AJ102" s="7">
+      <c r="AL102" s="7">
         <v>100</v>
       </c>
-      <c r="AK102" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL102" s="6">
+      <c r="AM102" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN102" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -14389,7 +14397,7 @@
         <v>34</v>
       </c>
       <c r="F103" s="10">
-        <f>29-COUNTIF(G103:AI103,8)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G103" s="7">
@@ -14479,17 +14487,17 @@
       <c r="AI103" s="7">
         <v>8</v>
       </c>
-      <c r="AJ103" s="7">
+      <c r="AL103" s="7">
         <v>100</v>
       </c>
-      <c r="AK103" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL103" s="6">
+      <c r="AM103" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN103" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -14506,7 +14514,7 @@
         <v>34</v>
       </c>
       <c r="F104" s="10">
-        <f>29-COUNTIF(G104:AI104,8)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G104" s="7">
@@ -14596,17 +14604,17 @@
       <c r="AI104" s="7">
         <v>8</v>
       </c>
-      <c r="AJ104" s="7">
+      <c r="AL104" s="7">
         <v>100</v>
       </c>
-      <c r="AK104" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL104" s="6">
+      <c r="AM104" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN104" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -14623,7 +14631,7 @@
         <v>34</v>
       </c>
       <c r="F105" s="10">
-        <f>29-COUNTIF(G105:AI105,8)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G105" s="7">
@@ -14713,17 +14721,17 @@
       <c r="AI105" s="7">
         <v>8</v>
       </c>
-      <c r="AJ105" s="7">
+      <c r="AL105" s="7">
         <v>100</v>
       </c>
-      <c r="AK105" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL105" s="6">
+      <c r="AM105" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN105" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -14740,7 +14748,7 @@
         <v>34</v>
       </c>
       <c r="F106" s="10">
-        <f>29-COUNTIF(G106:AI106,8)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G106" s="7">
@@ -14830,17 +14838,17 @@
       <c r="AI106" s="7">
         <v>8</v>
       </c>
-      <c r="AJ106" s="7">
+      <c r="AL106" s="7">
         <v>100</v>
       </c>
-      <c r="AK106" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL106" s="6">
+      <c r="AM106" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN106" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -14857,7 +14865,7 @@
         <v>34</v>
       </c>
       <c r="F107" s="10">
-        <f>29-COUNTIF(G107:AI107,8)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G107" s="7">
@@ -14947,17 +14955,17 @@
       <c r="AI107" s="7">
         <v>8</v>
       </c>
-      <c r="AJ107" s="7">
+      <c r="AL107" s="7">
         <v>100</v>
       </c>
-      <c r="AK107" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL107" s="6">
+      <c r="AM107" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN107" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -14974,7 +14982,7 @@
         <v>34</v>
       </c>
       <c r="F108" s="10">
-        <f>29-COUNTIF(G108:AI108,8)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G108" s="7">
@@ -15064,17 +15072,17 @@
       <c r="AI108" s="7">
         <v>8</v>
       </c>
-      <c r="AJ108" s="7">
+      <c r="AL108" s="7">
         <v>100</v>
       </c>
-      <c r="AK108" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL108" s="6">
+      <c r="AM108" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN108" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -15091,7 +15099,7 @@
         <v>34</v>
       </c>
       <c r="F109" s="10">
-        <f>29-COUNTIF(G109:AI109,8)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G109" s="7">
@@ -15181,17 +15189,17 @@
       <c r="AI109" s="7">
         <v>8</v>
       </c>
-      <c r="AJ109" s="7">
+      <c r="AL109" s="7">
         <v>100</v>
       </c>
-      <c r="AK109" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL109" s="6">
+      <c r="AM109" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN109" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -15208,7 +15216,7 @@
         <v>34</v>
       </c>
       <c r="F110" s="10">
-        <f>29-COUNTIF(G110:AI110,8)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G110" s="7">
@@ -15298,17 +15306,17 @@
       <c r="AI110" s="7">
         <v>8</v>
       </c>
-      <c r="AJ110" s="7">
+      <c r="AL110" s="7">
         <v>100</v>
       </c>
-      <c r="AK110" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL110" s="6">
+      <c r="AM110" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN110" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -15325,7 +15333,7 @@
         <v>34</v>
       </c>
       <c r="F111" s="10">
-        <f>29-COUNTIF(G111:AI111,8)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G111" s="7">
@@ -15415,17 +15423,17 @@
       <c r="AI111" s="7">
         <v>8</v>
       </c>
-      <c r="AJ111" s="7">
+      <c r="AL111" s="7">
         <v>100</v>
       </c>
-      <c r="AK111" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL111" s="6">
+      <c r="AM111" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN111" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -15442,7 +15450,7 @@
         <v>34</v>
       </c>
       <c r="F112" s="10">
-        <f>29-COUNTIF(G112:AI112,8)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G112" s="7">
@@ -15532,13 +15540,13 @@
       <c r="AI112" s="7">
         <v>8</v>
       </c>
-      <c r="AJ112" s="7">
+      <c r="AL112" s="7">
         <v>100</v>
       </c>
-      <c r="AK112" s="6">
-        <v>0</v>
-      </c>
-      <c r="AL112" s="6">
+      <c r="AM112" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN112" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>